<commit_message>
fix suffix in word file
</commit_message>
<xml_diff>
--- a/Реестр заявок №327.xlsx
+++ b/Реестр заявок №327.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <charset val="204"/>
@@ -43,8 +43,16 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -55,6 +63,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -123,10 +136,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -150,9 +164,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Нейтральный" xfId="1" builtinId="28"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
@@ -425,10 +444,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K422"/>
+  <dimension ref="A1:K423"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -669,11 +688,31 @@
       <c r="C7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="9" t="n"/>
-      <c r="E7" s="9" t="n"/>
-      <c r="F7" s="9" t="n"/>
-      <c r="G7" s="6" t="n"/>
-      <c r="H7" s="9" t="n"/>
+      <c r="D7" s="9" t="inlineStr">
+        <is>
+          <t>eqweqweqw</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="inlineStr">
+        <is>
+          <t>321123312</t>
+        </is>
+      </c>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>П-312321312</t>
+        </is>
+      </c>
+      <c r="G7" s="6" t="inlineStr">
+        <is>
+          <t>31.21.3232</t>
+        </is>
+      </c>
+      <c r="H7" s="9" t="inlineStr">
+        <is>
+          <t>Е.Р. Зотина</t>
+        </is>
+      </c>
       <c r="I7" s="1" t="n"/>
       <c r="J7" s="1" t="n"/>
     </row>
@@ -683,39 +722,77 @@
       <c r="C8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="n"/>
-      <c r="E8" s="9" t="n"/>
-      <c r="F8" s="9" t="n"/>
-      <c r="G8" s="6" t="n"/>
-      <c r="H8" s="9" t="n"/>
+      <c r="D8" s="9" t="inlineStr">
+        <is>
+          <t>dasdasdas</t>
+        </is>
+      </c>
+      <c r="E8" s="9" t="inlineStr">
+        <is>
+          <t>132123312</t>
+        </is>
+      </c>
+      <c r="F8" s="9" t="inlineStr">
+        <is>
+          <t>П-321132312132312</t>
+        </is>
+      </c>
+      <c r="G8" s="6" t="inlineStr">
+        <is>
+          <t>13.23.1231</t>
+        </is>
+      </c>
+      <c r="H8" s="9" t="inlineStr">
+        <is>
+          <t>Е.Р. Зотина</t>
+        </is>
+      </c>
       <c r="I8" s="1" t="n"/>
       <c r="J8" s="1" t="n"/>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="D9" s="9" t="n"/>
-      <c r="E9" s="9" t="n"/>
-      <c r="F9" s="9" t="n"/>
-      <c r="G9" s="6" t="n"/>
-      <c r="H9" s="9" t="n"/>
-      <c r="I9" s="1" t="n"/>
-      <c r="J9" s="1" t="n"/>
+    <row r="9" customFormat="1" s="18">
+      <c r="A9" s="15" t="n"/>
+      <c r="B9" s="15" t="n"/>
+      <c r="C9" s="15" t="n"/>
+      <c r="D9" s="16" t="n"/>
+      <c r="E9" s="16" t="n"/>
+      <c r="F9" s="16" t="n"/>
+      <c r="G9" s="17" t="n"/>
+      <c r="H9" s="16" t="n"/>
+      <c r="I9" s="15" t="n"/>
+      <c r="J9" s="15" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="n"/>
       <c r="C10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="D10" s="9" t="n"/>
-      <c r="E10" s="9" t="n"/>
-      <c r="F10" s="9" t="n"/>
-      <c r="G10" s="6" t="n"/>
-      <c r="H10" s="9" t="n"/>
+        <v>7</v>
+      </c>
+      <c r="D10" s="9" t="inlineStr">
+        <is>
+          <t>rwewerwre</t>
+        </is>
+      </c>
+      <c r="E10" s="9" t="inlineStr">
+        <is>
+          <t>423234423</t>
+        </is>
+      </c>
+      <c r="F10" s="9" t="inlineStr">
+        <is>
+          <t>П-234234342</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="inlineStr">
+        <is>
+          <t>23.42.3424</t>
+        </is>
+      </c>
+      <c r="H10" s="9" t="inlineStr">
+        <is>
+          <t>Е.Р. Зотина</t>
+        </is>
+      </c>
       <c r="I10" s="1" t="n"/>
       <c r="J10" s="1" t="n"/>
     </row>
@@ -723,13 +800,33 @@
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="n"/>
       <c r="C11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="D11" s="9" t="n"/>
-      <c r="E11" s="9" t="n"/>
-      <c r="F11" s="9" t="n"/>
-      <c r="G11" s="6" t="n"/>
-      <c r="H11" s="9" t="n"/>
+        <v>8</v>
+      </c>
+      <c r="D11" s="9" t="inlineStr">
+        <is>
+          <t>fsdfsddfs</t>
+        </is>
+      </c>
+      <c r="E11" s="9" t="inlineStr">
+        <is>
+          <t>312312231</t>
+        </is>
+      </c>
+      <c r="F11" s="9" t="inlineStr">
+        <is>
+          <t>П-312231132</t>
+        </is>
+      </c>
+      <c r="G11" s="6" t="inlineStr">
+        <is>
+          <t>13.22.3131</t>
+        </is>
+      </c>
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>Е.Р. Зотина</t>
+        </is>
+      </c>
       <c r="I11" s="1" t="n"/>
       <c r="J11" s="1" t="n"/>
     </row>
@@ -737,7 +834,7 @@
       <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="n"/>
       <c r="C12" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="9" t="n"/>
       <c r="E12" s="9" t="n"/>
@@ -751,7 +848,7 @@
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="9" t="n"/>
       <c r="E13" s="9" t="n"/>
@@ -765,7 +862,7 @@
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="n"/>
       <c r="C14" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="9" t="n"/>
       <c r="E14" s="9" t="n"/>
@@ -779,7 +876,7 @@
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="n"/>
       <c r="C15" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="9" t="n"/>
       <c r="E15" s="9" t="n"/>
@@ -793,7 +890,7 @@
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="n"/>
       <c r="C16" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="9" t="n"/>
       <c r="E16" s="9" t="n"/>
@@ -807,7 +904,7 @@
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="9" t="n"/>
       <c r="E17" s="9" t="n"/>
@@ -821,7 +918,7 @@
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="n"/>
       <c r="C18" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="9" t="n"/>
       <c r="E18" s="9" t="n"/>
@@ -835,7 +932,7 @@
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="n"/>
       <c r="C19" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="9" t="n"/>
       <c r="E19" s="9" t="n"/>
@@ -849,7 +946,7 @@
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="n"/>
       <c r="C20" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="9" t="n"/>
       <c r="E20" s="9" t="n"/>
@@ -863,7 +960,7 @@
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="n"/>
       <c r="C21" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="9" t="n"/>
       <c r="E21" s="9" t="n"/>
@@ -877,7 +974,7 @@
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="n"/>
       <c r="C22" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="9" t="n"/>
       <c r="E22" s="9" t="n"/>
@@ -891,7 +988,7 @@
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="9" t="n"/>
       <c r="E23" s="9" t="n"/>
@@ -905,7 +1002,7 @@
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="n"/>
       <c r="C24" s="1" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="9" t="n"/>
       <c r="E24" s="9" t="n"/>
@@ -919,7 +1016,7 @@
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="n"/>
       <c r="C25" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" s="9" t="n"/>
       <c r="E25" s="9" t="n"/>
@@ -933,7 +1030,7 @@
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="n"/>
       <c r="C26" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="9" t="n"/>
       <c r="E26" s="9" t="n"/>
@@ -947,7 +1044,7 @@
       <c r="A27" s="1" t="n"/>
       <c r="B27" s="1" t="n"/>
       <c r="C27" s="1" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" s="9" t="n"/>
       <c r="E27" s="9" t="n"/>
@@ -961,7 +1058,7 @@
       <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="n"/>
       <c r="C28" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" s="9" t="n"/>
       <c r="E28" s="9" t="n"/>
@@ -975,7 +1072,7 @@
       <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="n"/>
       <c r="C29" s="1" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="9" t="n"/>
       <c r="E29" s="9" t="n"/>
@@ -989,7 +1086,7 @@
       <c r="A30" s="1" t="n"/>
       <c r="B30" s="1" t="n"/>
       <c r="C30" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" s="9" t="n"/>
       <c r="E30" s="9" t="n"/>
@@ -1003,7 +1100,7 @@
       <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="n"/>
       <c r="C31" s="1" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="9" t="n"/>
       <c r="E31" s="9" t="n"/>
@@ -1017,7 +1114,7 @@
       <c r="A32" s="1" t="n"/>
       <c r="B32" s="1" t="n"/>
       <c r="C32" s="1" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="9" t="n"/>
       <c r="E32" s="9" t="n"/>
@@ -1031,7 +1128,7 @@
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="n"/>
       <c r="C33" s="1" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="9" t="n"/>
       <c r="E33" s="9" t="n"/>
@@ -1045,7 +1142,7 @@
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="n"/>
       <c r="C34" s="1" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="9" t="n"/>
       <c r="E34" s="9" t="n"/>
@@ -1059,7 +1156,7 @@
       <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="n"/>
       <c r="C35" s="1" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" s="9" t="n"/>
       <c r="E35" s="9" t="n"/>
@@ -1073,7 +1170,7 @@
       <c r="A36" s="1" t="n"/>
       <c r="B36" s="1" t="n"/>
       <c r="C36" s="1" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="9" t="n"/>
       <c r="E36" s="9" t="n"/>
@@ -1087,7 +1184,7 @@
       <c r="A37" s="1" t="n"/>
       <c r="B37" s="1" t="n"/>
       <c r="C37" s="1" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="9" t="n"/>
       <c r="E37" s="9" t="n"/>
@@ -1101,7 +1198,7 @@
       <c r="A38" s="1" t="n"/>
       <c r="B38" s="1" t="n"/>
       <c r="C38" s="1" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" s="9" t="n"/>
       <c r="E38" s="9" t="n"/>
@@ -1115,7 +1212,7 @@
       <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="n"/>
       <c r="C39" s="1" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" s="9" t="n"/>
       <c r="E39" s="9" t="n"/>
@@ -1129,7 +1226,7 @@
       <c r="A40" s="1" t="n"/>
       <c r="B40" s="1" t="n"/>
       <c r="C40" s="1" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" s="9" t="n"/>
       <c r="E40" s="9" t="n"/>
@@ -1143,7 +1240,7 @@
       <c r="A41" s="1" t="n"/>
       <c r="B41" s="1" t="n"/>
       <c r="C41" s="1" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" s="9" t="n"/>
       <c r="E41" s="9" t="n"/>
@@ -1157,7 +1254,7 @@
       <c r="A42" s="1" t="n"/>
       <c r="B42" s="1" t="n"/>
       <c r="C42" s="1" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" s="9" t="n"/>
       <c r="E42" s="9" t="n"/>
@@ -1171,7 +1268,7 @@
       <c r="A43" s="1" t="n"/>
       <c r="B43" s="1" t="n"/>
       <c r="C43" s="1" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D43" s="9" t="n"/>
       <c r="E43" s="9" t="n"/>
@@ -1185,7 +1282,7 @@
       <c r="A44" s="1" t="n"/>
       <c r="B44" s="1" t="n"/>
       <c r="C44" s="1" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D44" s="9" t="n"/>
       <c r="E44" s="9" t="n"/>
@@ -1199,7 +1296,7 @@
       <c r="A45" s="1" t="n"/>
       <c r="B45" s="1" t="n"/>
       <c r="C45" s="1" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D45" s="9" t="n"/>
       <c r="E45" s="9" t="n"/>
@@ -1213,7 +1310,7 @@
       <c r="A46" s="1" t="n"/>
       <c r="B46" s="1" t="n"/>
       <c r="C46" s="1" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" s="9" t="n"/>
       <c r="E46" s="9" t="n"/>
@@ -1227,7 +1324,7 @@
       <c r="A47" s="1" t="n"/>
       <c r="B47" s="1" t="n"/>
       <c r="C47" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D47" s="9" t="n"/>
       <c r="E47" s="9" t="n"/>
@@ -1241,7 +1338,7 @@
       <c r="A48" s="1" t="n"/>
       <c r="B48" s="1" t="n"/>
       <c r="C48" s="1" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D48" s="9" t="n"/>
       <c r="E48" s="9" t="n"/>
@@ -1255,7 +1352,7 @@
       <c r="A49" s="1" t="n"/>
       <c r="B49" s="1" t="n"/>
       <c r="C49" s="1" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" s="9" t="n"/>
       <c r="E49" s="9" t="n"/>
@@ -1269,7 +1366,7 @@
       <c r="A50" s="1" t="n"/>
       <c r="B50" s="1" t="n"/>
       <c r="C50" s="1" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D50" s="9" t="n"/>
       <c r="E50" s="9" t="n"/>
@@ -1283,7 +1380,7 @@
       <c r="A51" s="1" t="n"/>
       <c r="B51" s="1" t="n"/>
       <c r="C51" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" s="9" t="n"/>
       <c r="E51" s="9" t="n"/>
@@ -1297,7 +1394,7 @@
       <c r="A52" s="1" t="n"/>
       <c r="B52" s="1" t="n"/>
       <c r="C52" s="1" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D52" s="9" t="n"/>
       <c r="E52" s="9" t="n"/>
@@ -1311,7 +1408,7 @@
       <c r="A53" s="1" t="n"/>
       <c r="B53" s="1" t="n"/>
       <c r="C53" s="1" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D53" s="9" t="n"/>
       <c r="E53" s="9" t="n"/>
@@ -1325,7 +1422,7 @@
       <c r="A54" s="1" t="n"/>
       <c r="B54" s="1" t="n"/>
       <c r="C54" s="1" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" s="9" t="n"/>
       <c r="E54" s="9" t="n"/>
@@ -1339,7 +1436,7 @@
       <c r="A55" s="1" t="n"/>
       <c r="B55" s="1" t="n"/>
       <c r="C55" s="1" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D55" s="9" t="n"/>
       <c r="E55" s="9" t="n"/>
@@ -1353,7 +1450,7 @@
       <c r="A56" s="1" t="n"/>
       <c r="B56" s="1" t="n"/>
       <c r="C56" s="1" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D56" s="9" t="n"/>
       <c r="E56" s="9" t="n"/>
@@ -1367,7 +1464,7 @@
       <c r="A57" s="1" t="n"/>
       <c r="B57" s="1" t="n"/>
       <c r="C57" s="1" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57" s="9" t="n"/>
       <c r="E57" s="9" t="n"/>
@@ -1381,7 +1478,7 @@
       <c r="A58" s="1" t="n"/>
       <c r="B58" s="1" t="n"/>
       <c r="C58" s="1" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D58" s="9" t="n"/>
       <c r="E58" s="9" t="n"/>
@@ -1395,7 +1492,7 @@
       <c r="A59" s="1" t="n"/>
       <c r="B59" s="1" t="n"/>
       <c r="C59" s="1" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D59" s="9" t="n"/>
       <c r="E59" s="9" t="n"/>
@@ -1409,7 +1506,7 @@
       <c r="A60" s="1" t="n"/>
       <c r="B60" s="1" t="n"/>
       <c r="C60" s="1" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D60" s="9" t="n"/>
       <c r="E60" s="9" t="n"/>
@@ -1423,7 +1520,7 @@
       <c r="A61" s="1" t="n"/>
       <c r="B61" s="1" t="n"/>
       <c r="C61" s="1" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D61" s="9" t="n"/>
       <c r="E61" s="9" t="n"/>
@@ -1437,7 +1534,7 @@
       <c r="A62" s="1" t="n"/>
       <c r="B62" s="1" t="n"/>
       <c r="C62" s="1" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D62" s="9" t="n"/>
       <c r="E62" s="9" t="n"/>
@@ -1451,7 +1548,7 @@
       <c r="A63" s="1" t="n"/>
       <c r="B63" s="1" t="n"/>
       <c r="C63" s="1" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D63" s="9" t="n"/>
       <c r="E63" s="9" t="n"/>
@@ -1465,7 +1562,7 @@
       <c r="A64" s="1" t="n"/>
       <c r="B64" s="1" t="n"/>
       <c r="C64" s="1" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D64" s="9" t="n"/>
       <c r="E64" s="9" t="n"/>
@@ -1479,7 +1576,7 @@
       <c r="A65" s="1" t="n"/>
       <c r="B65" s="1" t="n"/>
       <c r="C65" s="1" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D65" s="9" t="n"/>
       <c r="E65" s="9" t="n"/>
@@ -1493,7 +1590,7 @@
       <c r="A66" s="1" t="n"/>
       <c r="B66" s="1" t="n"/>
       <c r="C66" s="1" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D66" s="9" t="n"/>
       <c r="E66" s="9" t="n"/>
@@ -1507,7 +1604,7 @@
       <c r="A67" s="1" t="n"/>
       <c r="B67" s="1" t="n"/>
       <c r="C67" s="1" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D67" s="9" t="n"/>
       <c r="E67" s="9" t="n"/>
@@ -1521,7 +1618,7 @@
       <c r="A68" s="1" t="n"/>
       <c r="B68" s="1" t="n"/>
       <c r="C68" s="1" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D68" s="9" t="n"/>
       <c r="E68" s="9" t="n"/>
@@ -1535,7 +1632,7 @@
       <c r="A69" s="1" t="n"/>
       <c r="B69" s="1" t="n"/>
       <c r="C69" s="1" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D69" s="9" t="n"/>
       <c r="E69" s="9" t="n"/>
@@ -1549,7 +1646,7 @@
       <c r="A70" s="1" t="n"/>
       <c r="B70" s="1" t="n"/>
       <c r="C70" s="1" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D70" s="9" t="n"/>
       <c r="E70" s="9" t="n"/>
@@ -1563,7 +1660,7 @@
       <c r="A71" s="1" t="n"/>
       <c r="B71" s="1" t="n"/>
       <c r="C71" s="1" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D71" s="9" t="n"/>
       <c r="E71" s="9" t="n"/>
@@ -1577,7 +1674,7 @@
       <c r="A72" s="1" t="n"/>
       <c r="B72" s="1" t="n"/>
       <c r="C72" s="1" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D72" s="9" t="n"/>
       <c r="E72" s="9" t="n"/>
@@ -1591,7 +1688,7 @@
       <c r="A73" s="1" t="n"/>
       <c r="B73" s="1" t="n"/>
       <c r="C73" s="1" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D73" s="9" t="n"/>
       <c r="E73" s="9" t="n"/>
@@ -1605,7 +1702,7 @@
       <c r="A74" s="1" t="n"/>
       <c r="B74" s="1" t="n"/>
       <c r="C74" s="1" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D74" s="9" t="n"/>
       <c r="E74" s="9" t="n"/>
@@ -1619,7 +1716,7 @@
       <c r="A75" s="1" t="n"/>
       <c r="B75" s="1" t="n"/>
       <c r="C75" s="1" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D75" s="9" t="n"/>
       <c r="E75" s="9" t="n"/>
@@ -1633,7 +1730,7 @@
       <c r="A76" s="1" t="n"/>
       <c r="B76" s="1" t="n"/>
       <c r="C76" s="1" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D76" s="9" t="n"/>
       <c r="E76" s="9" t="n"/>
@@ -1647,7 +1744,7 @@
       <c r="A77" s="1" t="n"/>
       <c r="B77" s="1" t="n"/>
       <c r="C77" s="1" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D77" s="9" t="n"/>
       <c r="E77" s="9" t="n"/>
@@ -1661,7 +1758,7 @@
       <c r="A78" s="1" t="n"/>
       <c r="B78" s="1" t="n"/>
       <c r="C78" s="1" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D78" s="9" t="n"/>
       <c r="E78" s="9" t="n"/>
@@ -1675,7 +1772,7 @@
       <c r="A79" s="1" t="n"/>
       <c r="B79" s="1" t="n"/>
       <c r="C79" s="1" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D79" s="9" t="n"/>
       <c r="E79" s="9" t="n"/>
@@ -1689,7 +1786,7 @@
       <c r="A80" s="1" t="n"/>
       <c r="B80" s="1" t="n"/>
       <c r="C80" s="1" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D80" s="9" t="n"/>
       <c r="E80" s="9" t="n"/>
@@ -1703,7 +1800,7 @@
       <c r="A81" s="1" t="n"/>
       <c r="B81" s="1" t="n"/>
       <c r="C81" s="1" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D81" s="9" t="n"/>
       <c r="E81" s="9" t="n"/>
@@ -1717,7 +1814,7 @@
       <c r="A82" s="1" t="n"/>
       <c r="B82" s="1" t="n"/>
       <c r="C82" s="1" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D82" s="9" t="n"/>
       <c r="E82" s="9" t="n"/>
@@ -1731,7 +1828,7 @@
       <c r="A83" s="1" t="n"/>
       <c r="B83" s="1" t="n"/>
       <c r="C83" s="1" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D83" s="9" t="n"/>
       <c r="E83" s="9" t="n"/>
@@ -1745,7 +1842,7 @@
       <c r="A84" s="1" t="n"/>
       <c r="B84" s="1" t="n"/>
       <c r="C84" s="1" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D84" s="9" t="n"/>
       <c r="E84" s="9" t="n"/>
@@ -1759,7 +1856,7 @@
       <c r="A85" s="1" t="n"/>
       <c r="B85" s="1" t="n"/>
       <c r="C85" s="1" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D85" s="9" t="n"/>
       <c r="E85" s="9" t="n"/>
@@ -1773,7 +1870,7 @@
       <c r="A86" s="1" t="n"/>
       <c r="B86" s="1" t="n"/>
       <c r="C86" s="1" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D86" s="9" t="n"/>
       <c r="E86" s="9" t="n"/>
@@ -1787,7 +1884,7 @@
       <c r="A87" s="1" t="n"/>
       <c r="B87" s="1" t="n"/>
       <c r="C87" s="1" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D87" s="9" t="n"/>
       <c r="E87" s="9" t="n"/>
@@ -1801,7 +1898,7 @@
       <c r="A88" s="1" t="n"/>
       <c r="B88" s="1" t="n"/>
       <c r="C88" s="1" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D88" s="9" t="n"/>
       <c r="E88" s="9" t="n"/>
@@ -1815,7 +1912,7 @@
       <c r="A89" s="1" t="n"/>
       <c r="B89" s="1" t="n"/>
       <c r="C89" s="1" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D89" s="9" t="n"/>
       <c r="E89" s="9" t="n"/>
@@ -1829,7 +1926,7 @@
       <c r="A90" s="1" t="n"/>
       <c r="B90" s="1" t="n"/>
       <c r="C90" s="1" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D90" s="9" t="n"/>
       <c r="E90" s="9" t="n"/>
@@ -1843,7 +1940,7 @@
       <c r="A91" s="1" t="n"/>
       <c r="B91" s="1" t="n"/>
       <c r="C91" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D91" s="9" t="n"/>
       <c r="E91" s="9" t="n"/>
@@ -1857,7 +1954,7 @@
       <c r="A92" s="1" t="n"/>
       <c r="B92" s="1" t="n"/>
       <c r="C92" s="1" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D92" s="9" t="n"/>
       <c r="E92" s="9" t="n"/>
@@ -1871,7 +1968,7 @@
       <c r="A93" s="1" t="n"/>
       <c r="B93" s="1" t="n"/>
       <c r="C93" s="1" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D93" s="9" t="n"/>
       <c r="E93" s="9" t="n"/>
@@ -1885,7 +1982,7 @@
       <c r="A94" s="1" t="n"/>
       <c r="B94" s="1" t="n"/>
       <c r="C94" s="1" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D94" s="9" t="n"/>
       <c r="E94" s="9" t="n"/>
@@ -1899,7 +1996,7 @@
       <c r="A95" s="1" t="n"/>
       <c r="B95" s="1" t="n"/>
       <c r="C95" s="1" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D95" s="9" t="n"/>
       <c r="E95" s="9" t="n"/>
@@ -1913,7 +2010,7 @@
       <c r="A96" s="1" t="n"/>
       <c r="B96" s="1" t="n"/>
       <c r="C96" s="1" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D96" s="9" t="n"/>
       <c r="E96" s="9" t="n"/>
@@ -1927,7 +2024,7 @@
       <c r="A97" s="1" t="n"/>
       <c r="B97" s="1" t="n"/>
       <c r="C97" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D97" s="9" t="n"/>
       <c r="E97" s="9" t="n"/>
@@ -1941,7 +2038,7 @@
       <c r="A98" s="1" t="n"/>
       <c r="B98" s="1" t="n"/>
       <c r="C98" s="1" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D98" s="9" t="n"/>
       <c r="E98" s="9" t="n"/>
@@ -1955,7 +2052,7 @@
       <c r="A99" s="1" t="n"/>
       <c r="B99" s="1" t="n"/>
       <c r="C99" s="1" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D99" s="9" t="n"/>
       <c r="E99" s="9" t="n"/>
@@ -1969,7 +2066,7 @@
       <c r="A100" s="1" t="n"/>
       <c r="B100" s="1" t="n"/>
       <c r="C100" s="1" t="n">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D100" s="9" t="n"/>
       <c r="E100" s="9" t="n"/>
@@ -1983,7 +2080,7 @@
       <c r="A101" s="1" t="n"/>
       <c r="B101" s="1" t="n"/>
       <c r="C101" s="1" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D101" s="9" t="n"/>
       <c r="E101" s="9" t="n"/>
@@ -1997,7 +2094,7 @@
       <c r="A102" s="1" t="n"/>
       <c r="B102" s="1" t="n"/>
       <c r="C102" s="1" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D102" s="9" t="n"/>
       <c r="E102" s="9" t="n"/>
@@ -2011,7 +2108,7 @@
       <c r="A103" s="1" t="n"/>
       <c r="B103" s="1" t="n"/>
       <c r="C103" s="1" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D103" s="9" t="n"/>
       <c r="E103" s="9" t="n"/>
@@ -2025,7 +2122,7 @@
       <c r="A104" s="1" t="n"/>
       <c r="B104" s="1" t="n"/>
       <c r="C104" s="1" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D104" s="9" t="n"/>
       <c r="E104" s="9" t="n"/>
@@ -2039,7 +2136,7 @@
       <c r="A105" s="1" t="n"/>
       <c r="B105" s="1" t="n"/>
       <c r="C105" s="1" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D105" s="9" t="n"/>
       <c r="E105" s="9" t="n"/>
@@ -2053,7 +2150,7 @@
       <c r="A106" s="1" t="n"/>
       <c r="B106" s="1" t="n"/>
       <c r="C106" s="1" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D106" s="9" t="n"/>
       <c r="E106" s="9" t="n"/>
@@ -2067,7 +2164,7 @@
       <c r="A107" s="1" t="n"/>
       <c r="B107" s="1" t="n"/>
       <c r="C107" s="1" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D107" s="9" t="n"/>
       <c r="E107" s="9" t="n"/>
@@ -2081,7 +2178,7 @@
       <c r="A108" s="1" t="n"/>
       <c r="B108" s="1" t="n"/>
       <c r="C108" s="1" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D108" s="9" t="n"/>
       <c r="E108" s="9" t="n"/>
@@ -2095,7 +2192,7 @@
       <c r="A109" s="1" t="n"/>
       <c r="B109" s="1" t="n"/>
       <c r="C109" s="1" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D109" s="9" t="n"/>
       <c r="E109" s="9" t="n"/>
@@ -2109,7 +2206,7 @@
       <c r="A110" s="1" t="n"/>
       <c r="B110" s="1" t="n"/>
       <c r="C110" s="1" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D110" s="9" t="n"/>
       <c r="E110" s="9" t="n"/>
@@ -2123,7 +2220,7 @@
       <c r="A111" s="1" t="n"/>
       <c r="B111" s="1" t="n"/>
       <c r="C111" s="1" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D111" s="9" t="n"/>
       <c r="E111" s="9" t="n"/>
@@ -2137,7 +2234,7 @@
       <c r="A112" s="1" t="n"/>
       <c r="B112" s="1" t="n"/>
       <c r="C112" s="1" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D112" s="9" t="n"/>
       <c r="E112" s="9" t="n"/>
@@ -2151,7 +2248,7 @@
       <c r="A113" s="1" t="n"/>
       <c r="B113" s="1" t="n"/>
       <c r="C113" s="1" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D113" s="9" t="n"/>
       <c r="E113" s="9" t="n"/>
@@ -2165,7 +2262,7 @@
       <c r="A114" s="1" t="n"/>
       <c r="B114" s="1" t="n"/>
       <c r="C114" s="1" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D114" s="9" t="n"/>
       <c r="E114" s="9" t="n"/>
@@ -2179,7 +2276,7 @@
       <c r="A115" s="1" t="n"/>
       <c r="B115" s="1" t="n"/>
       <c r="C115" s="1" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D115" s="9" t="n"/>
       <c r="E115" s="9" t="n"/>
@@ -2193,7 +2290,7 @@
       <c r="A116" s="1" t="n"/>
       <c r="B116" s="1" t="n"/>
       <c r="C116" s="1" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D116" s="9" t="n"/>
       <c r="E116" s="9" t="n"/>
@@ -2207,7 +2304,7 @@
       <c r="A117" s="1" t="n"/>
       <c r="B117" s="1" t="n"/>
       <c r="C117" s="1" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D117" s="9" t="n"/>
       <c r="E117" s="9" t="n"/>
@@ -2221,7 +2318,7 @@
       <c r="A118" s="1" t="n"/>
       <c r="B118" s="1" t="n"/>
       <c r="C118" s="1" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D118" s="9" t="n"/>
       <c r="E118" s="9" t="n"/>
@@ -2235,7 +2332,7 @@
       <c r="A119" s="1" t="n"/>
       <c r="B119" s="1" t="n"/>
       <c r="C119" s="1" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D119" s="9" t="n"/>
       <c r="E119" s="9" t="n"/>
@@ -2249,7 +2346,7 @@
       <c r="A120" s="1" t="n"/>
       <c r="B120" s="1" t="n"/>
       <c r="C120" s="1" t="n">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D120" s="9" t="n"/>
       <c r="E120" s="9" t="n"/>
@@ -2263,7 +2360,7 @@
       <c r="A121" s="1" t="n"/>
       <c r="B121" s="1" t="n"/>
       <c r="C121" s="1" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D121" s="9" t="n"/>
       <c r="E121" s="9" t="n"/>
@@ -2277,7 +2374,7 @@
       <c r="A122" s="1" t="n"/>
       <c r="B122" s="1" t="n"/>
       <c r="C122" s="1" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D122" s="9" t="n"/>
       <c r="E122" s="9" t="n"/>
@@ -2291,7 +2388,7 @@
       <c r="A123" s="1" t="n"/>
       <c r="B123" s="1" t="n"/>
       <c r="C123" s="1" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D123" s="9" t="n"/>
       <c r="E123" s="9" t="n"/>
@@ -2305,7 +2402,7 @@
       <c r="A124" s="1" t="n"/>
       <c r="B124" s="1" t="n"/>
       <c r="C124" s="1" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D124" s="9" t="n"/>
       <c r="E124" s="9" t="n"/>
@@ -2319,7 +2416,7 @@
       <c r="A125" s="1" t="n"/>
       <c r="B125" s="1" t="n"/>
       <c r="C125" s="1" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D125" s="9" t="n"/>
       <c r="E125" s="9" t="n"/>
@@ -2333,7 +2430,7 @@
       <c r="A126" s="1" t="n"/>
       <c r="B126" s="1" t="n"/>
       <c r="C126" s="1" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D126" s="9" t="n"/>
       <c r="E126" s="9" t="n"/>
@@ -2347,7 +2444,7 @@
       <c r="A127" s="1" t="n"/>
       <c r="B127" s="1" t="n"/>
       <c r="C127" s="1" t="n">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D127" s="9" t="n"/>
       <c r="E127" s="9" t="n"/>
@@ -2361,7 +2458,7 @@
       <c r="A128" s="1" t="n"/>
       <c r="B128" s="1" t="n"/>
       <c r="C128" s="1" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D128" s="9" t="n"/>
       <c r="E128" s="9" t="n"/>
@@ -2375,7 +2472,7 @@
       <c r="A129" s="1" t="n"/>
       <c r="B129" s="1" t="n"/>
       <c r="C129" s="1" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D129" s="9" t="n"/>
       <c r="E129" s="9" t="n"/>
@@ -2389,7 +2486,7 @@
       <c r="A130" s="1" t="n"/>
       <c r="B130" s="1" t="n"/>
       <c r="C130" s="1" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D130" s="9" t="n"/>
       <c r="E130" s="9" t="n"/>
@@ -2403,7 +2500,7 @@
       <c r="A131" s="1" t="n"/>
       <c r="B131" s="1" t="n"/>
       <c r="C131" s="1" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D131" s="9" t="n"/>
       <c r="E131" s="9" t="n"/>
@@ -2417,7 +2514,7 @@
       <c r="A132" s="1" t="n"/>
       <c r="B132" s="1" t="n"/>
       <c r="C132" s="1" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D132" s="9" t="n"/>
       <c r="E132" s="9" t="n"/>
@@ -2431,7 +2528,7 @@
       <c r="A133" s="1" t="n"/>
       <c r="B133" s="1" t="n"/>
       <c r="C133" s="1" t="n">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D133" s="9" t="n"/>
       <c r="E133" s="9" t="n"/>
@@ -2445,7 +2542,7 @@
       <c r="A134" s="1" t="n"/>
       <c r="B134" s="1" t="n"/>
       <c r="C134" s="1" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D134" s="9" t="n"/>
       <c r="E134" s="9" t="n"/>
@@ -2459,7 +2556,7 @@
       <c r="A135" s="1" t="n"/>
       <c r="B135" s="1" t="n"/>
       <c r="C135" s="1" t="n">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D135" s="9" t="n"/>
       <c r="E135" s="9" t="n"/>
@@ -2473,7 +2570,7 @@
       <c r="A136" s="1" t="n"/>
       <c r="B136" s="1" t="n"/>
       <c r="C136" s="1" t="n">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D136" s="9" t="n"/>
       <c r="E136" s="9" t="n"/>
@@ -2487,7 +2584,7 @@
       <c r="A137" s="1" t="n"/>
       <c r="B137" s="1" t="n"/>
       <c r="C137" s="1" t="n">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D137" s="9" t="n"/>
       <c r="E137" s="9" t="n"/>
@@ -2501,7 +2598,7 @@
       <c r="A138" s="1" t="n"/>
       <c r="B138" s="1" t="n"/>
       <c r="C138" s="1" t="n">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D138" s="9" t="n"/>
       <c r="E138" s="9" t="n"/>
@@ -2515,7 +2612,7 @@
       <c r="A139" s="1" t="n"/>
       <c r="B139" s="1" t="n"/>
       <c r="C139" s="1" t="n">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D139" s="9" t="n"/>
       <c r="E139" s="9" t="n"/>
@@ -2529,7 +2626,7 @@
       <c r="A140" s="1" t="n"/>
       <c r="B140" s="1" t="n"/>
       <c r="C140" s="1" t="n">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D140" s="9" t="n"/>
       <c r="E140" s="9" t="n"/>
@@ -2543,7 +2640,7 @@
       <c r="A141" s="1" t="n"/>
       <c r="B141" s="1" t="n"/>
       <c r="C141" s="1" t="n">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D141" s="9" t="n"/>
       <c r="E141" s="9" t="n"/>
@@ -2557,7 +2654,7 @@
       <c r="A142" s="1" t="n"/>
       <c r="B142" s="1" t="n"/>
       <c r="C142" s="1" t="n">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D142" s="9" t="n"/>
       <c r="E142" s="9" t="n"/>
@@ -2571,7 +2668,7 @@
       <c r="A143" s="1" t="n"/>
       <c r="B143" s="1" t="n"/>
       <c r="C143" s="1" t="n">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D143" s="9" t="n"/>
       <c r="E143" s="9" t="n"/>
@@ -2585,7 +2682,7 @@
       <c r="A144" s="1" t="n"/>
       <c r="B144" s="1" t="n"/>
       <c r="C144" s="1" t="n">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D144" s="9" t="n"/>
       <c r="E144" s="9" t="n"/>
@@ -2599,7 +2696,7 @@
       <c r="A145" s="1" t="n"/>
       <c r="B145" s="1" t="n"/>
       <c r="C145" s="1" t="n">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D145" s="9" t="n"/>
       <c r="E145" s="9" t="n"/>
@@ -2613,7 +2710,7 @@
       <c r="A146" s="1" t="n"/>
       <c r="B146" s="1" t="n"/>
       <c r="C146" s="1" t="n">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D146" s="9" t="n"/>
       <c r="E146" s="9" t="n"/>
@@ -2627,7 +2724,7 @@
       <c r="A147" s="1" t="n"/>
       <c r="B147" s="1" t="n"/>
       <c r="C147" s="1" t="n">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D147" s="9" t="n"/>
       <c r="E147" s="9" t="n"/>
@@ -2641,7 +2738,7 @@
       <c r="A148" s="1" t="n"/>
       <c r="B148" s="1" t="n"/>
       <c r="C148" s="1" t="n">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D148" s="9" t="n"/>
       <c r="E148" s="9" t="n"/>
@@ -2655,7 +2752,7 @@
       <c r="A149" s="1" t="n"/>
       <c r="B149" s="1" t="n"/>
       <c r="C149" s="1" t="n">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D149" s="9" t="n"/>
       <c r="E149" s="9" t="n"/>
@@ -2669,7 +2766,7 @@
       <c r="A150" s="1" t="n"/>
       <c r="B150" s="1" t="n"/>
       <c r="C150" s="1" t="n">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D150" s="9" t="n"/>
       <c r="E150" s="9" t="n"/>
@@ -2683,7 +2780,7 @@
       <c r="A151" s="1" t="n"/>
       <c r="B151" s="1" t="n"/>
       <c r="C151" s="1" t="n">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D151" s="9" t="n"/>
       <c r="E151" s="9" t="n"/>
@@ -2697,7 +2794,7 @@
       <c r="A152" s="1" t="n"/>
       <c r="B152" s="1" t="n"/>
       <c r="C152" s="1" t="n">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D152" s="9" t="n"/>
       <c r="E152" s="9" t="n"/>
@@ -2711,7 +2808,7 @@
       <c r="A153" s="1" t="n"/>
       <c r="B153" s="1" t="n"/>
       <c r="C153" s="1" t="n">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D153" s="9" t="n"/>
       <c r="E153" s="9" t="n"/>
@@ -2725,7 +2822,7 @@
       <c r="A154" s="1" t="n"/>
       <c r="B154" s="1" t="n"/>
       <c r="C154" s="1" t="n">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D154" s="9" t="n"/>
       <c r="E154" s="9" t="n"/>
@@ -2739,7 +2836,7 @@
       <c r="A155" s="1" t="n"/>
       <c r="B155" s="1" t="n"/>
       <c r="C155" s="1" t="n">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D155" s="9" t="n"/>
       <c r="E155" s="9" t="n"/>
@@ -2753,7 +2850,7 @@
       <c r="A156" s="1" t="n"/>
       <c r="B156" s="1" t="n"/>
       <c r="C156" s="1" t="n">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D156" s="9" t="n"/>
       <c r="E156" s="9" t="n"/>
@@ -2767,7 +2864,7 @@
       <c r="A157" s="1" t="n"/>
       <c r="B157" s="1" t="n"/>
       <c r="C157" s="1" t="n">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D157" s="9" t="n"/>
       <c r="E157" s="9" t="n"/>
@@ -2781,7 +2878,7 @@
       <c r="A158" s="1" t="n"/>
       <c r="B158" s="1" t="n"/>
       <c r="C158" s="1" t="n">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D158" s="9" t="n"/>
       <c r="E158" s="9" t="n"/>
@@ -2795,7 +2892,7 @@
       <c r="A159" s="1" t="n"/>
       <c r="B159" s="1" t="n"/>
       <c r="C159" s="1" t="n">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D159" s="9" t="n"/>
       <c r="E159" s="9" t="n"/>
@@ -2809,7 +2906,7 @@
       <c r="A160" s="1" t="n"/>
       <c r="B160" s="1" t="n"/>
       <c r="C160" s="1" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D160" s="9" t="n"/>
       <c r="E160" s="9" t="n"/>
@@ -2823,7 +2920,7 @@
       <c r="A161" s="1" t="n"/>
       <c r="B161" s="1" t="n"/>
       <c r="C161" s="1" t="n">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D161" s="9" t="n"/>
       <c r="E161" s="9" t="n"/>
@@ -2837,7 +2934,7 @@
       <c r="A162" s="1" t="n"/>
       <c r="B162" s="1" t="n"/>
       <c r="C162" s="1" t="n">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D162" s="9" t="n"/>
       <c r="E162" s="9" t="n"/>
@@ -2851,7 +2948,7 @@
       <c r="A163" s="1" t="n"/>
       <c r="B163" s="1" t="n"/>
       <c r="C163" s="1" t="n">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D163" s="9" t="n"/>
       <c r="E163" s="9" t="n"/>
@@ -2865,7 +2962,7 @@
       <c r="A164" s="1" t="n"/>
       <c r="B164" s="1" t="n"/>
       <c r="C164" s="1" t="n">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D164" s="9" t="n"/>
       <c r="E164" s="9" t="n"/>
@@ -2879,7 +2976,7 @@
       <c r="A165" s="1" t="n"/>
       <c r="B165" s="1" t="n"/>
       <c r="C165" s="1" t="n">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D165" s="9" t="n"/>
       <c r="E165" s="9" t="n"/>
@@ -2893,7 +2990,7 @@
       <c r="A166" s="1" t="n"/>
       <c r="B166" s="1" t="n"/>
       <c r="C166" s="1" t="n">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D166" s="9" t="n"/>
       <c r="E166" s="9" t="n"/>
@@ -2907,7 +3004,7 @@
       <c r="A167" s="1" t="n"/>
       <c r="B167" s="1" t="n"/>
       <c r="C167" s="1" t="n">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D167" s="9" t="n"/>
       <c r="E167" s="9" t="n"/>
@@ -2921,7 +3018,7 @@
       <c r="A168" s="1" t="n"/>
       <c r="B168" s="1" t="n"/>
       <c r="C168" s="1" t="n">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D168" s="9" t="n"/>
       <c r="E168" s="9" t="n"/>
@@ -2935,7 +3032,7 @@
       <c r="A169" s="1" t="n"/>
       <c r="B169" s="1" t="n"/>
       <c r="C169" s="1" t="n">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D169" s="9" t="n"/>
       <c r="E169" s="9" t="n"/>
@@ -2949,7 +3046,7 @@
       <c r="A170" s="1" t="n"/>
       <c r="B170" s="1" t="n"/>
       <c r="C170" s="1" t="n">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D170" s="9" t="n"/>
       <c r="E170" s="9" t="n"/>
@@ -2963,7 +3060,7 @@
       <c r="A171" s="1" t="n"/>
       <c r="B171" s="1" t="n"/>
       <c r="C171" s="1" t="n">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D171" s="9" t="n"/>
       <c r="E171" s="9" t="n"/>
@@ -2977,7 +3074,7 @@
       <c r="A172" s="1" t="n"/>
       <c r="B172" s="1" t="n"/>
       <c r="C172" s="1" t="n">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D172" s="9" t="n"/>
       <c r="E172" s="9" t="n"/>
@@ -2991,7 +3088,7 @@
       <c r="A173" s="1" t="n"/>
       <c r="B173" s="1" t="n"/>
       <c r="C173" s="1" t="n">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D173" s="9" t="n"/>
       <c r="E173" s="9" t="n"/>
@@ -3005,7 +3102,7 @@
       <c r="A174" s="1" t="n"/>
       <c r="B174" s="1" t="n"/>
       <c r="C174" s="1" t="n">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D174" s="9" t="n"/>
       <c r="E174" s="9" t="n"/>
@@ -3019,7 +3116,7 @@
       <c r="A175" s="1" t="n"/>
       <c r="B175" s="1" t="n"/>
       <c r="C175" s="1" t="n">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D175" s="9" t="n"/>
       <c r="E175" s="9" t="n"/>
@@ -3033,7 +3130,7 @@
       <c r="A176" s="1" t="n"/>
       <c r="B176" s="1" t="n"/>
       <c r="C176" s="1" t="n">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D176" s="9" t="n"/>
       <c r="E176" s="9" t="n"/>
@@ -3047,7 +3144,7 @@
       <c r="A177" s="1" t="n"/>
       <c r="B177" s="1" t="n"/>
       <c r="C177" s="1" t="n">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D177" s="9" t="n"/>
       <c r="E177" s="9" t="n"/>
@@ -3061,7 +3158,7 @@
       <c r="A178" s="1" t="n"/>
       <c r="B178" s="1" t="n"/>
       <c r="C178" s="1" t="n">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D178" s="9" t="n"/>
       <c r="E178" s="9" t="n"/>
@@ -3075,7 +3172,7 @@
       <c r="A179" s="1" t="n"/>
       <c r="B179" s="1" t="n"/>
       <c r="C179" s="1" t="n">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D179" s="9" t="n"/>
       <c r="E179" s="9" t="n"/>
@@ -3089,7 +3186,7 @@
       <c r="A180" s="1" t="n"/>
       <c r="B180" s="1" t="n"/>
       <c r="C180" s="1" t="n">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D180" s="9" t="n"/>
       <c r="E180" s="9" t="n"/>
@@ -3103,7 +3200,7 @@
       <c r="A181" s="1" t="n"/>
       <c r="B181" s="1" t="n"/>
       <c r="C181" s="1" t="n">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D181" s="9" t="n"/>
       <c r="E181" s="9" t="n"/>
@@ -3117,7 +3214,7 @@
       <c r="A182" s="1" t="n"/>
       <c r="B182" s="1" t="n"/>
       <c r="C182" s="1" t="n">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D182" s="9" t="n"/>
       <c r="E182" s="9" t="n"/>
@@ -3131,7 +3228,7 @@
       <c r="A183" s="1" t="n"/>
       <c r="B183" s="1" t="n"/>
       <c r="C183" s="1" t="n">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D183" s="9" t="n"/>
       <c r="E183" s="9" t="n"/>
@@ -3145,7 +3242,7 @@
       <c r="A184" s="1" t="n"/>
       <c r="B184" s="1" t="n"/>
       <c r="C184" s="1" t="n">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D184" s="9" t="n"/>
       <c r="E184" s="9" t="n"/>
@@ -3159,7 +3256,7 @@
       <c r="A185" s="1" t="n"/>
       <c r="B185" s="1" t="n"/>
       <c r="C185" s="1" t="n">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D185" s="9" t="n"/>
       <c r="E185" s="9" t="n"/>
@@ -3173,7 +3270,7 @@
       <c r="A186" s="1" t="n"/>
       <c r="B186" s="1" t="n"/>
       <c r="C186" s="1" t="n">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D186" s="9" t="n"/>
       <c r="E186" s="9" t="n"/>
@@ -3187,7 +3284,7 @@
       <c r="A187" s="1" t="n"/>
       <c r="B187" s="1" t="n"/>
       <c r="C187" s="1" t="n">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D187" s="9" t="n"/>
       <c r="E187" s="9" t="n"/>
@@ -3201,7 +3298,7 @@
       <c r="A188" s="1" t="n"/>
       <c r="B188" s="1" t="n"/>
       <c r="C188" s="1" t="n">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D188" s="9" t="n"/>
       <c r="E188" s="9" t="n"/>
@@ -3215,7 +3312,7 @@
       <c r="A189" s="1" t="n"/>
       <c r="B189" s="1" t="n"/>
       <c r="C189" s="1" t="n">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D189" s="9" t="n"/>
       <c r="E189" s="9" t="n"/>
@@ -3229,7 +3326,7 @@
       <c r="A190" s="1" t="n"/>
       <c r="B190" s="1" t="n"/>
       <c r="C190" s="1" t="n">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D190" s="9" t="n"/>
       <c r="E190" s="9" t="n"/>
@@ -3243,7 +3340,7 @@
       <c r="A191" s="1" t="n"/>
       <c r="B191" s="1" t="n"/>
       <c r="C191" s="1" t="n">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D191" s="9" t="n"/>
       <c r="E191" s="9" t="n"/>
@@ -3257,7 +3354,7 @@
       <c r="A192" s="1" t="n"/>
       <c r="B192" s="1" t="n"/>
       <c r="C192" s="1" t="n">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D192" s="9" t="n"/>
       <c r="E192" s="9" t="n"/>
@@ -3271,7 +3368,7 @@
       <c r="A193" s="1" t="n"/>
       <c r="B193" s="1" t="n"/>
       <c r="C193" s="1" t="n">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D193" s="9" t="n"/>
       <c r="E193" s="9" t="n"/>
@@ -3285,7 +3382,7 @@
       <c r="A194" s="1" t="n"/>
       <c r="B194" s="1" t="n"/>
       <c r="C194" s="1" t="n">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D194" s="9" t="n"/>
       <c r="E194" s="9" t="n"/>
@@ -3299,7 +3396,7 @@
       <c r="A195" s="1" t="n"/>
       <c r="B195" s="1" t="n"/>
       <c r="C195" s="1" t="n">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D195" s="9" t="n"/>
       <c r="E195" s="9" t="n"/>
@@ -3313,7 +3410,7 @@
       <c r="A196" s="1" t="n"/>
       <c r="B196" s="1" t="n"/>
       <c r="C196" s="1" t="n">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D196" s="9" t="n"/>
       <c r="E196" s="9" t="n"/>
@@ -3327,7 +3424,7 @@
       <c r="A197" s="1" t="n"/>
       <c r="B197" s="1" t="n"/>
       <c r="C197" s="1" t="n">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D197" s="9" t="n"/>
       <c r="E197" s="9" t="n"/>
@@ -3341,7 +3438,7 @@
       <c r="A198" s="1" t="n"/>
       <c r="B198" s="1" t="n"/>
       <c r="C198" s="1" t="n">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D198" s="9" t="n"/>
       <c r="E198" s="9" t="n"/>
@@ -3355,7 +3452,7 @@
       <c r="A199" s="1" t="n"/>
       <c r="B199" s="1" t="n"/>
       <c r="C199" s="1" t="n">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D199" s="9" t="n"/>
       <c r="E199" s="9" t="n"/>
@@ -3369,7 +3466,7 @@
       <c r="A200" s="1" t="n"/>
       <c r="B200" s="1" t="n"/>
       <c r="C200" s="1" t="n">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D200" s="9" t="n"/>
       <c r="E200" s="9" t="n"/>
@@ -3383,7 +3480,7 @@
       <c r="A201" s="1" t="n"/>
       <c r="B201" s="1" t="n"/>
       <c r="C201" s="1" t="n">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D201" s="9" t="n"/>
       <c r="E201" s="9" t="n"/>
@@ -3397,7 +3494,7 @@
       <c r="A202" s="1" t="n"/>
       <c r="B202" s="1" t="n"/>
       <c r="C202" s="1" t="n">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D202" s="9" t="n"/>
       <c r="E202" s="9" t="n"/>
@@ -3411,7 +3508,7 @@
       <c r="A203" s="1" t="n"/>
       <c r="B203" s="1" t="n"/>
       <c r="C203" s="1" t="n">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D203" s="9" t="n"/>
       <c r="E203" s="9" t="n"/>
@@ -3425,7 +3522,7 @@
       <c r="A204" s="1" t="n"/>
       <c r="B204" s="1" t="n"/>
       <c r="C204" s="1" t="n">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D204" s="9" t="n"/>
       <c r="E204" s="9" t="n"/>
@@ -3439,7 +3536,7 @@
       <c r="A205" s="1" t="n"/>
       <c r="B205" s="1" t="n"/>
       <c r="C205" s="1" t="n">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D205" s="9" t="n"/>
       <c r="E205" s="9" t="n"/>
@@ -3453,7 +3550,7 @@
       <c r="A206" s="1" t="n"/>
       <c r="B206" s="1" t="n"/>
       <c r="C206" s="1" t="n">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D206" s="9" t="n"/>
       <c r="E206" s="9" t="n"/>
@@ -3467,7 +3564,7 @@
       <c r="A207" s="1" t="n"/>
       <c r="B207" s="1" t="n"/>
       <c r="C207" s="1" t="n">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D207" s="9" t="n"/>
       <c r="E207" s="9" t="n"/>
@@ -3481,7 +3578,7 @@
       <c r="A208" s="1" t="n"/>
       <c r="B208" s="1" t="n"/>
       <c r="C208" s="1" t="n">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D208" s="9" t="n"/>
       <c r="E208" s="9" t="n"/>
@@ -3495,7 +3592,7 @@
       <c r="A209" s="1" t="n"/>
       <c r="B209" s="1" t="n"/>
       <c r="C209" s="1" t="n">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D209" s="9" t="n"/>
       <c r="E209" s="9" t="n"/>
@@ -3509,7 +3606,7 @@
       <c r="A210" s="1" t="n"/>
       <c r="B210" s="1" t="n"/>
       <c r="C210" s="1" t="n">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D210" s="9" t="n"/>
       <c r="E210" s="9" t="n"/>
@@ -3523,7 +3620,7 @@
       <c r="A211" s="1" t="n"/>
       <c r="B211" s="1" t="n"/>
       <c r="C211" s="1" t="n">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D211" s="9" t="n"/>
       <c r="E211" s="9" t="n"/>
@@ -3537,7 +3634,7 @@
       <c r="A212" s="1" t="n"/>
       <c r="B212" s="1" t="n"/>
       <c r="C212" s="1" t="n">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D212" s="9" t="n"/>
       <c r="E212" s="9" t="n"/>
@@ -3551,7 +3648,7 @@
       <c r="A213" s="1" t="n"/>
       <c r="B213" s="1" t="n"/>
       <c r="C213" s="1" t="n">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D213" s="9" t="n"/>
       <c r="E213" s="9" t="n"/>
@@ -3565,7 +3662,7 @@
       <c r="A214" s="1" t="n"/>
       <c r="B214" s="1" t="n"/>
       <c r="C214" s="1" t="n">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D214" s="9" t="n"/>
       <c r="E214" s="9" t="n"/>
@@ -3579,7 +3676,7 @@
       <c r="A215" s="1" t="n"/>
       <c r="B215" s="1" t="n"/>
       <c r="C215" s="1" t="n">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D215" s="9" t="n"/>
       <c r="E215" s="9" t="n"/>
@@ -3593,7 +3690,7 @@
       <c r="A216" s="1" t="n"/>
       <c r="B216" s="1" t="n"/>
       <c r="C216" s="1" t="n">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D216" s="9" t="n"/>
       <c r="E216" s="9" t="n"/>
@@ -3607,7 +3704,7 @@
       <c r="A217" s="1" t="n"/>
       <c r="B217" s="1" t="n"/>
       <c r="C217" s="1" t="n">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D217" s="9" t="n"/>
       <c r="E217" s="9" t="n"/>
@@ -3621,7 +3718,7 @@
       <c r="A218" s="1" t="n"/>
       <c r="B218" s="1" t="n"/>
       <c r="C218" s="1" t="n">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D218" s="9" t="n"/>
       <c r="E218" s="9" t="n"/>
@@ -3635,7 +3732,7 @@
       <c r="A219" s="1" t="n"/>
       <c r="B219" s="1" t="n"/>
       <c r="C219" s="1" t="n">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D219" s="9" t="n"/>
       <c r="E219" s="9" t="n"/>
@@ -3649,7 +3746,7 @@
       <c r="A220" s="1" t="n"/>
       <c r="B220" s="1" t="n"/>
       <c r="C220" s="1" t="n">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D220" s="9" t="n"/>
       <c r="E220" s="9" t="n"/>
@@ -3663,7 +3760,7 @@
       <c r="A221" s="1" t="n"/>
       <c r="B221" s="1" t="n"/>
       <c r="C221" s="1" t="n">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D221" s="9" t="n"/>
       <c r="E221" s="9" t="n"/>
@@ -3677,7 +3774,7 @@
       <c r="A222" s="1" t="n"/>
       <c r="B222" s="1" t="n"/>
       <c r="C222" s="1" t="n">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D222" s="9" t="n"/>
       <c r="E222" s="9" t="n"/>
@@ -3691,7 +3788,7 @@
       <c r="A223" s="1" t="n"/>
       <c r="B223" s="1" t="n"/>
       <c r="C223" s="1" t="n">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D223" s="9" t="n"/>
       <c r="E223" s="9" t="n"/>
@@ -3705,7 +3802,7 @@
       <c r="A224" s="1" t="n"/>
       <c r="B224" s="1" t="n"/>
       <c r="C224" s="1" t="n">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D224" s="9" t="n"/>
       <c r="E224" s="9" t="n"/>
@@ -3719,7 +3816,7 @@
       <c r="A225" s="1" t="n"/>
       <c r="B225" s="1" t="n"/>
       <c r="C225" s="1" t="n">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D225" s="9" t="n"/>
       <c r="E225" s="9" t="n"/>
@@ -3733,7 +3830,7 @@
       <c r="A226" s="1" t="n"/>
       <c r="B226" s="1" t="n"/>
       <c r="C226" s="1" t="n">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D226" s="9" t="n"/>
       <c r="E226" s="9" t="n"/>
@@ -3747,7 +3844,7 @@
       <c r="A227" s="1" t="n"/>
       <c r="B227" s="1" t="n"/>
       <c r="C227" s="1" t="n">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D227" s="9" t="n"/>
       <c r="E227" s="9" t="n"/>
@@ -3761,7 +3858,7 @@
       <c r="A228" s="1" t="n"/>
       <c r="B228" s="1" t="n"/>
       <c r="C228" s="1" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D228" s="9" t="n"/>
       <c r="E228" s="9" t="n"/>
@@ -3775,7 +3872,7 @@
       <c r="A229" s="1" t="n"/>
       <c r="B229" s="1" t="n"/>
       <c r="C229" s="1" t="n">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D229" s="9" t="n"/>
       <c r="E229" s="9" t="n"/>
@@ -3789,7 +3886,7 @@
       <c r="A230" s="1" t="n"/>
       <c r="B230" s="1" t="n"/>
       <c r="C230" s="1" t="n">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D230" s="9" t="n"/>
       <c r="E230" s="9" t="n"/>
@@ -3803,7 +3900,7 @@
       <c r="A231" s="1" t="n"/>
       <c r="B231" s="1" t="n"/>
       <c r="C231" s="1" t="n">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D231" s="9" t="n"/>
       <c r="E231" s="9" t="n"/>
@@ -3817,7 +3914,7 @@
       <c r="A232" s="1" t="n"/>
       <c r="B232" s="1" t="n"/>
       <c r="C232" s="1" t="n">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D232" s="9" t="n"/>
       <c r="E232" s="9" t="n"/>
@@ -3831,7 +3928,7 @@
       <c r="A233" s="1" t="n"/>
       <c r="B233" s="1" t="n"/>
       <c r="C233" s="1" t="n">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D233" s="9" t="n"/>
       <c r="E233" s="9" t="n"/>
@@ -3845,7 +3942,7 @@
       <c r="A234" s="1" t="n"/>
       <c r="B234" s="1" t="n"/>
       <c r="C234" s="1" t="n">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D234" s="9" t="n"/>
       <c r="E234" s="9" t="n"/>
@@ -3859,7 +3956,7 @@
       <c r="A235" s="1" t="n"/>
       <c r="B235" s="1" t="n"/>
       <c r="C235" s="1" t="n">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D235" s="9" t="n"/>
       <c r="E235" s="9" t="n"/>
@@ -3873,7 +3970,7 @@
       <c r="A236" s="1" t="n"/>
       <c r="B236" s="1" t="n"/>
       <c r="C236" s="1" t="n">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D236" s="9" t="n"/>
       <c r="E236" s="9" t="n"/>
@@ -3887,7 +3984,7 @@
       <c r="A237" s="1" t="n"/>
       <c r="B237" s="1" t="n"/>
       <c r="C237" s="1" t="n">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D237" s="9" t="n"/>
       <c r="E237" s="9" t="n"/>
@@ -3901,7 +3998,7 @@
       <c r="A238" s="1" t="n"/>
       <c r="B238" s="1" t="n"/>
       <c r="C238" s="1" t="n">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D238" s="9" t="n"/>
       <c r="E238" s="9" t="n"/>
@@ -3915,7 +4012,7 @@
       <c r="A239" s="1" t="n"/>
       <c r="B239" s="1" t="n"/>
       <c r="C239" s="1" t="n">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D239" s="9" t="n"/>
       <c r="E239" s="9" t="n"/>
@@ -3929,7 +4026,7 @@
       <c r="A240" s="1" t="n"/>
       <c r="B240" s="1" t="n"/>
       <c r="C240" s="1" t="n">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D240" s="9" t="n"/>
       <c r="E240" s="9" t="n"/>
@@ -3943,7 +4040,7 @@
       <c r="A241" s="1" t="n"/>
       <c r="B241" s="1" t="n"/>
       <c r="C241" s="1" t="n">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D241" s="9" t="n"/>
       <c r="E241" s="9" t="n"/>
@@ -3957,7 +4054,7 @@
       <c r="A242" s="1" t="n"/>
       <c r="B242" s="1" t="n"/>
       <c r="C242" s="1" t="n">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D242" s="9" t="n"/>
       <c r="E242" s="9" t="n"/>
@@ -3971,7 +4068,7 @@
       <c r="A243" s="1" t="n"/>
       <c r="B243" s="1" t="n"/>
       <c r="C243" s="1" t="n">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D243" s="9" t="n"/>
       <c r="E243" s="9" t="n"/>
@@ -3985,7 +4082,7 @@
       <c r="A244" s="1" t="n"/>
       <c r="B244" s="1" t="n"/>
       <c r="C244" s="1" t="n">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D244" s="9" t="n"/>
       <c r="E244" s="9" t="n"/>
@@ -3999,7 +4096,7 @@
       <c r="A245" s="1" t="n"/>
       <c r="B245" s="1" t="n"/>
       <c r="C245" s="1" t="n">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D245" s="9" t="n"/>
       <c r="E245" s="9" t="n"/>
@@ -4013,7 +4110,7 @@
       <c r="A246" s="1" t="n"/>
       <c r="B246" s="1" t="n"/>
       <c r="C246" s="1" t="n">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D246" s="9" t="n"/>
       <c r="E246" s="9" t="n"/>
@@ -4027,7 +4124,7 @@
       <c r="A247" s="1" t="n"/>
       <c r="B247" s="1" t="n"/>
       <c r="C247" s="1" t="n">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D247" s="9" t="n"/>
       <c r="E247" s="9" t="n"/>
@@ -4041,7 +4138,7 @@
       <c r="A248" s="1" t="n"/>
       <c r="B248" s="1" t="n"/>
       <c r="C248" s="1" t="n">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D248" s="9" t="n"/>
       <c r="E248" s="9" t="n"/>
@@ -4055,7 +4152,7 @@
       <c r="A249" s="1" t="n"/>
       <c r="B249" s="1" t="n"/>
       <c r="C249" s="1" t="n">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D249" s="9" t="n"/>
       <c r="E249" s="9" t="n"/>
@@ -4069,7 +4166,7 @@
       <c r="A250" s="1" t="n"/>
       <c r="B250" s="1" t="n"/>
       <c r="C250" s="1" t="n">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D250" s="9" t="n"/>
       <c r="E250" s="9" t="n"/>
@@ -4083,7 +4180,7 @@
       <c r="A251" s="1" t="n"/>
       <c r="B251" s="1" t="n"/>
       <c r="C251" s="1" t="n">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D251" s="9" t="n"/>
       <c r="E251" s="9" t="n"/>
@@ -4097,7 +4194,7 @@
       <c r="A252" s="1" t="n"/>
       <c r="B252" s="1" t="n"/>
       <c r="C252" s="1" t="n">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D252" s="9" t="n"/>
       <c r="E252" s="9" t="n"/>
@@ -4111,7 +4208,7 @@
       <c r="A253" s="1" t="n"/>
       <c r="B253" s="1" t="n"/>
       <c r="C253" s="1" t="n">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D253" s="9" t="n"/>
       <c r="E253" s="9" t="n"/>
@@ -4125,7 +4222,7 @@
       <c r="A254" s="1" t="n"/>
       <c r="B254" s="1" t="n"/>
       <c r="C254" s="1" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D254" s="9" t="n"/>
       <c r="E254" s="9" t="n"/>
@@ -4139,7 +4236,7 @@
       <c r="A255" s="1" t="n"/>
       <c r="B255" s="1" t="n"/>
       <c r="C255" s="1" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D255" s="9" t="n"/>
       <c r="E255" s="9" t="n"/>
@@ -4153,7 +4250,7 @@
       <c r="A256" s="1" t="n"/>
       <c r="B256" s="1" t="n"/>
       <c r="C256" s="1" t="n">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D256" s="9" t="n"/>
       <c r="E256" s="9" t="n"/>
@@ -4167,7 +4264,7 @@
       <c r="A257" s="1" t="n"/>
       <c r="B257" s="1" t="n"/>
       <c r="C257" s="1" t="n">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D257" s="9" t="n"/>
       <c r="E257" s="9" t="n"/>
@@ -4181,7 +4278,7 @@
       <c r="A258" s="1" t="n"/>
       <c r="B258" s="1" t="n"/>
       <c r="C258" s="1" t="n">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D258" s="9" t="n"/>
       <c r="E258" s="9" t="n"/>
@@ -4195,7 +4292,7 @@
       <c r="A259" s="1" t="n"/>
       <c r="B259" s="1" t="n"/>
       <c r="C259" s="1" t="n">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D259" s="9" t="n"/>
       <c r="E259" s="9" t="n"/>
@@ -4209,7 +4306,7 @@
       <c r="A260" s="1" t="n"/>
       <c r="B260" s="1" t="n"/>
       <c r="C260" s="1" t="n">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D260" s="9" t="n"/>
       <c r="E260" s="9" t="n"/>
@@ -4223,7 +4320,7 @@
       <c r="A261" s="1" t="n"/>
       <c r="B261" s="1" t="n"/>
       <c r="C261" s="1" t="n">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D261" s="9" t="n"/>
       <c r="E261" s="9" t="n"/>
@@ -4237,7 +4334,7 @@
       <c r="A262" s="1" t="n"/>
       <c r="B262" s="1" t="n"/>
       <c r="C262" s="1" t="n">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D262" s="9" t="n"/>
       <c r="E262" s="9" t="n"/>
@@ -4251,7 +4348,7 @@
       <c r="A263" s="1" t="n"/>
       <c r="B263" s="1" t="n"/>
       <c r="C263" s="1" t="n">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D263" s="9" t="n"/>
       <c r="E263" s="9" t="n"/>
@@ -4265,7 +4362,7 @@
       <c r="A264" s="1" t="n"/>
       <c r="B264" s="1" t="n"/>
       <c r="C264" s="1" t="n">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D264" s="9" t="n"/>
       <c r="E264" s="9" t="n"/>
@@ -4279,7 +4376,7 @@
       <c r="A265" s="1" t="n"/>
       <c r="B265" s="1" t="n"/>
       <c r="C265" s="1" t="n">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D265" s="9" t="n"/>
       <c r="E265" s="9" t="n"/>
@@ -4293,7 +4390,7 @@
       <c r="A266" s="1" t="n"/>
       <c r="B266" s="1" t="n"/>
       <c r="C266" s="1" t="n">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D266" s="9" t="n"/>
       <c r="E266" s="9" t="n"/>
@@ -4307,7 +4404,7 @@
       <c r="A267" s="1" t="n"/>
       <c r="B267" s="1" t="n"/>
       <c r="C267" s="1" t="n">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D267" s="9" t="n"/>
       <c r="E267" s="9" t="n"/>
@@ -4321,7 +4418,7 @@
       <c r="A268" s="1" t="n"/>
       <c r="B268" s="1" t="n"/>
       <c r="C268" s="1" t="n">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D268" s="9" t="n"/>
       <c r="E268" s="9" t="n"/>
@@ -4335,7 +4432,7 @@
       <c r="A269" s="1" t="n"/>
       <c r="B269" s="1" t="n"/>
       <c r="C269" s="1" t="n">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D269" s="9" t="n"/>
       <c r="E269" s="9" t="n"/>
@@ -4349,7 +4446,7 @@
       <c r="A270" s="1" t="n"/>
       <c r="B270" s="1" t="n"/>
       <c r="C270" s="1" t="n">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D270" s="9" t="n"/>
       <c r="E270" s="9" t="n"/>
@@ -4363,7 +4460,7 @@
       <c r="A271" s="1" t="n"/>
       <c r="B271" s="1" t="n"/>
       <c r="C271" s="1" t="n">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D271" s="9" t="n"/>
       <c r="E271" s="9" t="n"/>
@@ -4377,7 +4474,7 @@
       <c r="A272" s="1" t="n"/>
       <c r="B272" s="1" t="n"/>
       <c r="C272" s="1" t="n">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D272" s="9" t="n"/>
       <c r="E272" s="9" t="n"/>
@@ -4391,7 +4488,7 @@
       <c r="A273" s="1" t="n"/>
       <c r="B273" s="1" t="n"/>
       <c r="C273" s="1" t="n">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D273" s="9" t="n"/>
       <c r="E273" s="9" t="n"/>
@@ -4405,7 +4502,7 @@
       <c r="A274" s="1" t="n"/>
       <c r="B274" s="1" t="n"/>
       <c r="C274" s="1" t="n">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D274" s="9" t="n"/>
       <c r="E274" s="9" t="n"/>
@@ -4419,7 +4516,7 @@
       <c r="A275" s="1" t="n"/>
       <c r="B275" s="1" t="n"/>
       <c r="C275" s="1" t="n">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D275" s="9" t="n"/>
       <c r="E275" s="9" t="n"/>
@@ -4433,7 +4530,7 @@
       <c r="A276" s="1" t="n"/>
       <c r="B276" s="1" t="n"/>
       <c r="C276" s="1" t="n">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D276" s="9" t="n"/>
       <c r="E276" s="9" t="n"/>
@@ -4447,7 +4544,7 @@
       <c r="A277" s="1" t="n"/>
       <c r="B277" s="1" t="n"/>
       <c r="C277" s="1" t="n">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D277" s="9" t="n"/>
       <c r="E277" s="9" t="n"/>
@@ -4461,7 +4558,7 @@
       <c r="A278" s="1" t="n"/>
       <c r="B278" s="1" t="n"/>
       <c r="C278" s="1" t="n">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D278" s="9" t="n"/>
       <c r="E278" s="9" t="n"/>
@@ -4475,7 +4572,7 @@
       <c r="A279" s="1" t="n"/>
       <c r="B279" s="1" t="n"/>
       <c r="C279" s="1" t="n">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D279" s="9" t="n"/>
       <c r="E279" s="9" t="n"/>
@@ -4489,7 +4586,7 @@
       <c r="A280" s="1" t="n"/>
       <c r="B280" s="1" t="n"/>
       <c r="C280" s="1" t="n">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D280" s="9" t="n"/>
       <c r="E280" s="9" t="n"/>
@@ -4503,7 +4600,7 @@
       <c r="A281" s="1" t="n"/>
       <c r="B281" s="1" t="n"/>
       <c r="C281" s="1" t="n">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D281" s="9" t="n"/>
       <c r="E281" s="9" t="n"/>
@@ -4517,7 +4614,7 @@
       <c r="A282" s="1" t="n"/>
       <c r="B282" s="1" t="n"/>
       <c r="C282" s="1" t="n">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D282" s="9" t="n"/>
       <c r="E282" s="9" t="n"/>
@@ -4531,7 +4628,7 @@
       <c r="A283" s="1" t="n"/>
       <c r="B283" s="1" t="n"/>
       <c r="C283" s="1" t="n">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D283" s="9" t="n"/>
       <c r="E283" s="9" t="n"/>
@@ -4545,7 +4642,7 @@
       <c r="A284" s="1" t="n"/>
       <c r="B284" s="1" t="n"/>
       <c r="C284" s="1" t="n">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D284" s="9" t="n"/>
       <c r="E284" s="9" t="n"/>
@@ -4559,7 +4656,7 @@
       <c r="A285" s="1" t="n"/>
       <c r="B285" s="1" t="n"/>
       <c r="C285" s="1" t="n">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D285" s="9" t="n"/>
       <c r="E285" s="9" t="n"/>
@@ -4573,7 +4670,7 @@
       <c r="A286" s="1" t="n"/>
       <c r="B286" s="1" t="n"/>
       <c r="C286" s="1" t="n">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D286" s="9" t="n"/>
       <c r="E286" s="9" t="n"/>
@@ -4587,7 +4684,7 @@
       <c r="A287" s="1" t="n"/>
       <c r="B287" s="1" t="n"/>
       <c r="C287" s="1" t="n">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D287" s="9" t="n"/>
       <c r="E287" s="9" t="n"/>
@@ -4601,7 +4698,7 @@
       <c r="A288" s="1" t="n"/>
       <c r="B288" s="1" t="n"/>
       <c r="C288" s="1" t="n">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D288" s="9" t="n"/>
       <c r="E288" s="9" t="n"/>
@@ -4615,7 +4712,7 @@
       <c r="A289" s="1" t="n"/>
       <c r="B289" s="1" t="n"/>
       <c r="C289" s="1" t="n">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D289" s="9" t="n"/>
       <c r="E289" s="9" t="n"/>
@@ -4629,7 +4726,7 @@
       <c r="A290" s="1" t="n"/>
       <c r="B290" s="1" t="n"/>
       <c r="C290" s="1" t="n">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D290" s="9" t="n"/>
       <c r="E290" s="9" t="n"/>
@@ -4643,7 +4740,7 @@
       <c r="A291" s="1" t="n"/>
       <c r="B291" s="1" t="n"/>
       <c r="C291" s="1" t="n">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D291" s="9" t="n"/>
       <c r="E291" s="9" t="n"/>
@@ -4657,7 +4754,7 @@
       <c r="A292" s="1" t="n"/>
       <c r="B292" s="1" t="n"/>
       <c r="C292" s="1" t="n">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D292" s="9" t="n"/>
       <c r="E292" s="9" t="n"/>
@@ -4671,7 +4768,7 @@
       <c r="A293" s="1" t="n"/>
       <c r="B293" s="1" t="n"/>
       <c r="C293" s="1" t="n">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D293" s="9" t="n"/>
       <c r="E293" s="9" t="n"/>
@@ -4685,7 +4782,7 @@
       <c r="A294" s="1" t="n"/>
       <c r="B294" s="1" t="n"/>
       <c r="C294" s="1" t="n">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D294" s="9" t="n"/>
       <c r="E294" s="9" t="n"/>
@@ -4699,7 +4796,7 @@
       <c r="A295" s="1" t="n"/>
       <c r="B295" s="1" t="n"/>
       <c r="C295" s="1" t="n">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D295" s="9" t="n"/>
       <c r="E295" s="9" t="n"/>
@@ -4713,7 +4810,7 @@
       <c r="A296" s="1" t="n"/>
       <c r="B296" s="1" t="n"/>
       <c r="C296" s="1" t="n">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D296" s="9" t="n"/>
       <c r="E296" s="9" t="n"/>
@@ -4727,7 +4824,7 @@
       <c r="A297" s="1" t="n"/>
       <c r="B297" s="1" t="n"/>
       <c r="C297" s="1" t="n">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D297" s="9" t="n"/>
       <c r="E297" s="9" t="n"/>
@@ -4741,7 +4838,7 @@
       <c r="A298" s="1" t="n"/>
       <c r="B298" s="1" t="n"/>
       <c r="C298" s="1" t="n">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D298" s="9" t="n"/>
       <c r="E298" s="9" t="n"/>
@@ -4755,7 +4852,7 @@
       <c r="A299" s="1" t="n"/>
       <c r="B299" s="1" t="n"/>
       <c r="C299" s="1" t="n">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D299" s="9" t="n"/>
       <c r="E299" s="9" t="n"/>
@@ -4769,7 +4866,7 @@
       <c r="A300" s="1" t="n"/>
       <c r="B300" s="1" t="n"/>
       <c r="C300" s="1" t="n">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D300" s="9" t="n"/>
       <c r="E300" s="9" t="n"/>
@@ -4783,7 +4880,7 @@
       <c r="A301" s="1" t="n"/>
       <c r="B301" s="1" t="n"/>
       <c r="C301" s="1" t="n">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D301" s="9" t="n"/>
       <c r="E301" s="9" t="n"/>
@@ -4797,7 +4894,7 @@
       <c r="A302" s="1" t="n"/>
       <c r="B302" s="1" t="n"/>
       <c r="C302" s="1" t="n">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D302" s="9" t="n"/>
       <c r="E302" s="9" t="n"/>
@@ -4811,7 +4908,7 @@
       <c r="A303" s="1" t="n"/>
       <c r="B303" s="1" t="n"/>
       <c r="C303" s="1" t="n">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D303" s="9" t="n"/>
       <c r="E303" s="9" t="n"/>
@@ -4825,7 +4922,7 @@
       <c r="A304" s="1" t="n"/>
       <c r="B304" s="1" t="n"/>
       <c r="C304" s="1" t="n">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D304" s="9" t="n"/>
       <c r="E304" s="9" t="n"/>
@@ -4839,7 +4936,7 @@
       <c r="A305" s="1" t="n"/>
       <c r="B305" s="1" t="n"/>
       <c r="C305" s="1" t="n">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D305" s="9" t="n"/>
       <c r="E305" s="9" t="n"/>
@@ -4853,7 +4950,7 @@
       <c r="A306" s="1" t="n"/>
       <c r="B306" s="1" t="n"/>
       <c r="C306" s="1" t="n">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D306" s="9" t="n"/>
       <c r="E306" s="9" t="n"/>
@@ -4867,7 +4964,7 @@
       <c r="A307" s="1" t="n"/>
       <c r="B307" s="1" t="n"/>
       <c r="C307" s="1" t="n">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D307" s="9" t="n"/>
       <c r="E307" s="9" t="n"/>
@@ -4881,7 +4978,7 @@
       <c r="A308" s="1" t="n"/>
       <c r="B308" s="1" t="n"/>
       <c r="C308" s="1" t="n">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D308" s="9" t="n"/>
       <c r="E308" s="9" t="n"/>
@@ -4895,7 +4992,7 @@
       <c r="A309" s="1" t="n"/>
       <c r="B309" s="1" t="n"/>
       <c r="C309" s="1" t="n">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D309" s="9" t="n"/>
       <c r="E309" s="9" t="n"/>
@@ -4909,7 +5006,7 @@
       <c r="A310" s="1" t="n"/>
       <c r="B310" s="1" t="n"/>
       <c r="C310" s="1" t="n">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D310" s="9" t="n"/>
       <c r="E310" s="9" t="n"/>
@@ -4923,7 +5020,7 @@
       <c r="A311" s="1" t="n"/>
       <c r="B311" s="1" t="n"/>
       <c r="C311" s="1" t="n">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D311" s="9" t="n"/>
       <c r="E311" s="9" t="n"/>
@@ -4937,7 +5034,7 @@
       <c r="A312" s="1" t="n"/>
       <c r="B312" s="1" t="n"/>
       <c r="C312" s="1" t="n">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D312" s="9" t="n"/>
       <c r="E312" s="9" t="n"/>
@@ -4951,7 +5048,7 @@
       <c r="A313" s="1" t="n"/>
       <c r="B313" s="1" t="n"/>
       <c r="C313" s="1" t="n">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D313" s="9" t="n"/>
       <c r="E313" s="9" t="n"/>
@@ -4965,7 +5062,7 @@
       <c r="A314" s="1" t="n"/>
       <c r="B314" s="1" t="n"/>
       <c r="C314" s="1" t="n">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D314" s="9" t="n"/>
       <c r="E314" s="9" t="n"/>
@@ -4979,7 +5076,7 @@
       <c r="A315" s="1" t="n"/>
       <c r="B315" s="1" t="n"/>
       <c r="C315" s="1" t="n">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D315" s="9" t="n"/>
       <c r="E315" s="9" t="n"/>
@@ -4993,7 +5090,7 @@
       <c r="A316" s="1" t="n"/>
       <c r="B316" s="1" t="n"/>
       <c r="C316" s="1" t="n">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D316" s="9" t="n"/>
       <c r="E316" s="9" t="n"/>
@@ -5007,7 +5104,7 @@
       <c r="A317" s="1" t="n"/>
       <c r="B317" s="1" t="n"/>
       <c r="C317" s="1" t="n">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D317" s="9" t="n"/>
       <c r="E317" s="9" t="n"/>
@@ -5021,7 +5118,7 @@
       <c r="A318" s="1" t="n"/>
       <c r="B318" s="1" t="n"/>
       <c r="C318" s="1" t="n">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D318" s="9" t="n"/>
       <c r="E318" s="9" t="n"/>
@@ -5035,7 +5132,7 @@
       <c r="A319" s="1" t="n"/>
       <c r="B319" s="1" t="n"/>
       <c r="C319" s="1" t="n">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D319" s="9" t="n"/>
       <c r="E319" s="9" t="n"/>
@@ -5049,7 +5146,7 @@
       <c r="A320" s="1" t="n"/>
       <c r="B320" s="1" t="n"/>
       <c r="C320" s="1" t="n">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D320" s="9" t="n"/>
       <c r="E320" s="9" t="n"/>
@@ -5063,7 +5160,7 @@
       <c r="A321" s="1" t="n"/>
       <c r="B321" s="1" t="n"/>
       <c r="C321" s="1" t="n">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D321" s="9" t="n"/>
       <c r="E321" s="9" t="n"/>
@@ -5077,7 +5174,7 @@
       <c r="A322" s="1" t="n"/>
       <c r="B322" s="1" t="n"/>
       <c r="C322" s="1" t="n">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D322" s="9" t="n"/>
       <c r="E322" s="9" t="n"/>
@@ -5091,7 +5188,7 @@
       <c r="A323" s="1" t="n"/>
       <c r="B323" s="1" t="n"/>
       <c r="C323" s="1" t="n">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D323" s="9" t="n"/>
       <c r="E323" s="9" t="n"/>
@@ -5105,7 +5202,7 @@
       <c r="A324" s="1" t="n"/>
       <c r="B324" s="1" t="n"/>
       <c r="C324" s="1" t="n">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D324" s="9" t="n"/>
       <c r="E324" s="9" t="n"/>
@@ -5119,7 +5216,7 @@
       <c r="A325" s="1" t="n"/>
       <c r="B325" s="1" t="n"/>
       <c r="C325" s="1" t="n">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D325" s="9" t="n"/>
       <c r="E325" s="9" t="n"/>
@@ -5133,7 +5230,7 @@
       <c r="A326" s="1" t="n"/>
       <c r="B326" s="1" t="n"/>
       <c r="C326" s="1" t="n">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D326" s="9" t="n"/>
       <c r="E326" s="9" t="n"/>
@@ -5147,7 +5244,7 @@
       <c r="A327" s="1" t="n"/>
       <c r="B327" s="1" t="n"/>
       <c r="C327" s="1" t="n">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D327" s="9" t="n"/>
       <c r="E327" s="9" t="n"/>
@@ -5161,7 +5258,7 @@
       <c r="A328" s="1" t="n"/>
       <c r="B328" s="1" t="n"/>
       <c r="C328" s="1" t="n">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D328" s="9" t="n"/>
       <c r="E328" s="9" t="n"/>
@@ -5175,7 +5272,7 @@
       <c r="A329" s="1" t="n"/>
       <c r="B329" s="1" t="n"/>
       <c r="C329" s="1" t="n">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D329" s="9" t="n"/>
       <c r="E329" s="9" t="n"/>
@@ -5189,7 +5286,7 @@
       <c r="A330" s="1" t="n"/>
       <c r="B330" s="1" t="n"/>
       <c r="C330" s="1" t="n">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D330" s="9" t="n"/>
       <c r="E330" s="9" t="n"/>
@@ -5203,7 +5300,7 @@
       <c r="A331" s="1" t="n"/>
       <c r="B331" s="1" t="n"/>
       <c r="C331" s="1" t="n">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D331" s="9" t="n"/>
       <c r="E331" s="9" t="n"/>
@@ -5217,7 +5314,7 @@
       <c r="A332" s="1" t="n"/>
       <c r="B332" s="1" t="n"/>
       <c r="C332" s="1" t="n">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D332" s="9" t="n"/>
       <c r="E332" s="9" t="n"/>
@@ -5231,7 +5328,7 @@
       <c r="A333" s="1" t="n"/>
       <c r="B333" s="1" t="n"/>
       <c r="C333" s="1" t="n">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D333" s="9" t="n"/>
       <c r="E333" s="9" t="n"/>
@@ -5245,7 +5342,7 @@
       <c r="A334" s="1" t="n"/>
       <c r="B334" s="1" t="n"/>
       <c r="C334" s="1" t="n">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D334" s="9" t="n"/>
       <c r="E334" s="9" t="n"/>
@@ -5259,7 +5356,7 @@
       <c r="A335" s="1" t="n"/>
       <c r="B335" s="1" t="n"/>
       <c r="C335" s="1" t="n">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D335" s="9" t="n"/>
       <c r="E335" s="9" t="n"/>
@@ -5273,7 +5370,7 @@
       <c r="A336" s="1" t="n"/>
       <c r="B336" s="1" t="n"/>
       <c r="C336" s="1" t="n">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D336" s="9" t="n"/>
       <c r="E336" s="9" t="n"/>
@@ -5287,7 +5384,7 @@
       <c r="A337" s="1" t="n"/>
       <c r="B337" s="1" t="n"/>
       <c r="C337" s="1" t="n">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D337" s="9" t="n"/>
       <c r="E337" s="9" t="n"/>
@@ -5301,7 +5398,7 @@
       <c r="A338" s="1" t="n"/>
       <c r="B338" s="1" t="n"/>
       <c r="C338" s="1" t="n">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D338" s="9" t="n"/>
       <c r="E338" s="9" t="n"/>
@@ -5315,7 +5412,7 @@
       <c r="A339" s="1" t="n"/>
       <c r="B339" s="1" t="n"/>
       <c r="C339" s="1" t="n">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D339" s="9" t="n"/>
       <c r="E339" s="9" t="n"/>
@@ -5329,7 +5426,7 @@
       <c r="A340" s="1" t="n"/>
       <c r="B340" s="1" t="n"/>
       <c r="C340" s="1" t="n">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D340" s="9" t="n"/>
       <c r="E340" s="9" t="n"/>
@@ -5343,7 +5440,7 @@
       <c r="A341" s="1" t="n"/>
       <c r="B341" s="1" t="n"/>
       <c r="C341" s="1" t="n">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D341" s="9" t="n"/>
       <c r="E341" s="9" t="n"/>
@@ -5357,7 +5454,7 @@
       <c r="A342" s="1" t="n"/>
       <c r="B342" s="1" t="n"/>
       <c r="C342" s="1" t="n">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D342" s="9" t="n"/>
       <c r="E342" s="9" t="n"/>
@@ -5371,7 +5468,7 @@
       <c r="A343" s="1" t="n"/>
       <c r="B343" s="1" t="n"/>
       <c r="C343" s="1" t="n">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D343" s="9" t="n"/>
       <c r="E343" s="9" t="n"/>
@@ -5385,7 +5482,7 @@
       <c r="A344" s="1" t="n"/>
       <c r="B344" s="1" t="n"/>
       <c r="C344" s="1" t="n">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D344" s="9" t="n"/>
       <c r="E344" s="9" t="n"/>
@@ -5399,7 +5496,7 @@
       <c r="A345" s="1" t="n"/>
       <c r="B345" s="1" t="n"/>
       <c r="C345" s="1" t="n">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D345" s="9" t="n"/>
       <c r="E345" s="9" t="n"/>
@@ -5413,7 +5510,7 @@
       <c r="A346" s="1" t="n"/>
       <c r="B346" s="1" t="n"/>
       <c r="C346" s="1" t="n">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D346" s="9" t="n"/>
       <c r="E346" s="9" t="n"/>
@@ -5427,7 +5524,7 @@
       <c r="A347" s="1" t="n"/>
       <c r="B347" s="1" t="n"/>
       <c r="C347" s="1" t="n">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D347" s="9" t="n"/>
       <c r="E347" s="9" t="n"/>
@@ -5441,7 +5538,7 @@
       <c r="A348" s="1" t="n"/>
       <c r="B348" s="1" t="n"/>
       <c r="C348" s="1" t="n">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D348" s="9" t="n"/>
       <c r="E348" s="9" t="n"/>
@@ -5455,7 +5552,7 @@
       <c r="A349" s="1" t="n"/>
       <c r="B349" s="1" t="n"/>
       <c r="C349" s="1" t="n">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D349" s="9" t="n"/>
       <c r="E349" s="9" t="n"/>
@@ -5469,7 +5566,7 @@
       <c r="A350" s="1" t="n"/>
       <c r="B350" s="1" t="n"/>
       <c r="C350" s="1" t="n">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D350" s="9" t="n"/>
       <c r="E350" s="9" t="n"/>
@@ -5483,7 +5580,7 @@
       <c r="A351" s="1" t="n"/>
       <c r="B351" s="1" t="n"/>
       <c r="C351" s="1" t="n">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D351" s="9" t="n"/>
       <c r="E351" s="9" t="n"/>
@@ -5497,7 +5594,7 @@
       <c r="A352" s="1" t="n"/>
       <c r="B352" s="1" t="n"/>
       <c r="C352" s="1" t="n">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D352" s="9" t="n"/>
       <c r="E352" s="9" t="n"/>
@@ -5511,7 +5608,7 @@
       <c r="A353" s="1" t="n"/>
       <c r="B353" s="1" t="n"/>
       <c r="C353" s="1" t="n">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D353" s="9" t="n"/>
       <c r="E353" s="9" t="n"/>
@@ -5525,7 +5622,7 @@
       <c r="A354" s="1" t="n"/>
       <c r="B354" s="1" t="n"/>
       <c r="C354" s="1" t="n">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D354" s="9" t="n"/>
       <c r="E354" s="9" t="n"/>
@@ -5539,7 +5636,7 @@
       <c r="A355" s="1" t="n"/>
       <c r="B355" s="1" t="n"/>
       <c r="C355" s="1" t="n">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D355" s="9" t="n"/>
       <c r="E355" s="9" t="n"/>
@@ -5553,7 +5650,7 @@
       <c r="A356" s="1" t="n"/>
       <c r="B356" s="1" t="n"/>
       <c r="C356" s="1" t="n">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D356" s="9" t="n"/>
       <c r="E356" s="9" t="n"/>
@@ -5567,7 +5664,7 @@
       <c r="A357" s="1" t="n"/>
       <c r="B357" s="1" t="n"/>
       <c r="C357" s="1" t="n">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D357" s="9" t="n"/>
       <c r="E357" s="9" t="n"/>
@@ -5581,7 +5678,7 @@
       <c r="A358" s="1" t="n"/>
       <c r="B358" s="1" t="n"/>
       <c r="C358" s="1" t="n">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D358" s="9" t="n"/>
       <c r="E358" s="9" t="n"/>
@@ -5595,7 +5692,7 @@
       <c r="A359" s="1" t="n"/>
       <c r="B359" s="1" t="n"/>
       <c r="C359" s="1" t="n">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D359" s="9" t="n"/>
       <c r="E359" s="9" t="n"/>
@@ -5609,7 +5706,7 @@
       <c r="A360" s="1" t="n"/>
       <c r="B360" s="1" t="n"/>
       <c r="C360" s="1" t="n">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D360" s="9" t="n"/>
       <c r="E360" s="9" t="n"/>
@@ -5623,7 +5720,7 @@
       <c r="A361" s="1" t="n"/>
       <c r="B361" s="1" t="n"/>
       <c r="C361" s="1" t="n">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D361" s="9" t="n"/>
       <c r="E361" s="9" t="n"/>
@@ -5637,7 +5734,7 @@
       <c r="A362" s="1" t="n"/>
       <c r="B362" s="1" t="n"/>
       <c r="C362" s="1" t="n">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D362" s="9" t="n"/>
       <c r="E362" s="9" t="n"/>
@@ -5651,7 +5748,7 @@
       <c r="A363" s="1" t="n"/>
       <c r="B363" s="1" t="n"/>
       <c r="C363" s="1" t="n">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D363" s="9" t="n"/>
       <c r="E363" s="9" t="n"/>
@@ -5665,7 +5762,7 @@
       <c r="A364" s="1" t="n"/>
       <c r="B364" s="1" t="n"/>
       <c r="C364" s="1" t="n">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D364" s="9" t="n"/>
       <c r="E364" s="9" t="n"/>
@@ -5679,7 +5776,7 @@
       <c r="A365" s="1" t="n"/>
       <c r="B365" s="1" t="n"/>
       <c r="C365" s="1" t="n">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D365" s="9" t="n"/>
       <c r="E365" s="9" t="n"/>
@@ -5693,7 +5790,7 @@
       <c r="A366" s="1" t="n"/>
       <c r="B366" s="1" t="n"/>
       <c r="C366" s="1" t="n">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D366" s="9" t="n"/>
       <c r="E366" s="9" t="n"/>
@@ -5707,7 +5804,7 @@
       <c r="A367" s="1" t="n"/>
       <c r="B367" s="1" t="n"/>
       <c r="C367" s="1" t="n">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D367" s="9" t="n"/>
       <c r="E367" s="9" t="n"/>
@@ -5721,7 +5818,7 @@
       <c r="A368" s="1" t="n"/>
       <c r="B368" s="1" t="n"/>
       <c r="C368" s="1" t="n">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D368" s="9" t="n"/>
       <c r="E368" s="9" t="n"/>
@@ -5735,7 +5832,7 @@
       <c r="A369" s="1" t="n"/>
       <c r="B369" s="1" t="n"/>
       <c r="C369" s="1" t="n">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D369" s="9" t="n"/>
       <c r="E369" s="9" t="n"/>
@@ -5749,7 +5846,7 @@
       <c r="A370" s="1" t="n"/>
       <c r="B370" s="1" t="n"/>
       <c r="C370" s="1" t="n">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D370" s="9" t="n"/>
       <c r="E370" s="9" t="n"/>
@@ -5763,7 +5860,7 @@
       <c r="A371" s="1" t="n"/>
       <c r="B371" s="1" t="n"/>
       <c r="C371" s="1" t="n">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D371" s="9" t="n"/>
       <c r="E371" s="9" t="n"/>
@@ -5777,7 +5874,7 @@
       <c r="A372" s="1" t="n"/>
       <c r="B372" s="1" t="n"/>
       <c r="C372" s="1" t="n">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D372" s="9" t="n"/>
       <c r="E372" s="9" t="n"/>
@@ -5791,7 +5888,7 @@
       <c r="A373" s="1" t="n"/>
       <c r="B373" s="1" t="n"/>
       <c r="C373" s="1" t="n">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D373" s="9" t="n"/>
       <c r="E373" s="9" t="n"/>
@@ -5805,7 +5902,7 @@
       <c r="A374" s="1" t="n"/>
       <c r="B374" s="1" t="n"/>
       <c r="C374" s="1" t="n">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D374" s="9" t="n"/>
       <c r="E374" s="9" t="n"/>
@@ -5819,7 +5916,7 @@
       <c r="A375" s="1" t="n"/>
       <c r="B375" s="1" t="n"/>
       <c r="C375" s="1" t="n">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D375" s="9" t="n"/>
       <c r="E375" s="9" t="n"/>
@@ -5833,7 +5930,7 @@
       <c r="A376" s="1" t="n"/>
       <c r="B376" s="1" t="n"/>
       <c r="C376" s="1" t="n">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D376" s="9" t="n"/>
       <c r="E376" s="9" t="n"/>
@@ -5847,7 +5944,7 @@
       <c r="A377" s="1" t="n"/>
       <c r="B377" s="1" t="n"/>
       <c r="C377" s="1" t="n">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D377" s="9" t="n"/>
       <c r="E377" s="9" t="n"/>
@@ -5861,7 +5958,7 @@
       <c r="A378" s="1" t="n"/>
       <c r="B378" s="1" t="n"/>
       <c r="C378" s="1" t="n">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D378" s="9" t="n"/>
       <c r="E378" s="9" t="n"/>
@@ -5875,7 +5972,7 @@
       <c r="A379" s="1" t="n"/>
       <c r="B379" s="1" t="n"/>
       <c r="C379" s="1" t="n">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D379" s="9" t="n"/>
       <c r="E379" s="9" t="n"/>
@@ -5889,7 +5986,7 @@
       <c r="A380" s="1" t="n"/>
       <c r="B380" s="1" t="n"/>
       <c r="C380" s="1" t="n">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D380" s="9" t="n"/>
       <c r="E380" s="9" t="n"/>
@@ -5903,7 +6000,7 @@
       <c r="A381" s="1" t="n"/>
       <c r="B381" s="1" t="n"/>
       <c r="C381" s="1" t="n">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D381" s="9" t="n"/>
       <c r="E381" s="9" t="n"/>
@@ -5917,7 +6014,7 @@
       <c r="A382" s="1" t="n"/>
       <c r="B382" s="1" t="n"/>
       <c r="C382" s="1" t="n">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D382" s="9" t="n"/>
       <c r="E382" s="9" t="n"/>
@@ -5931,7 +6028,7 @@
       <c r="A383" s="1" t="n"/>
       <c r="B383" s="1" t="n"/>
       <c r="C383" s="1" t="n">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D383" s="9" t="n"/>
       <c r="E383" s="9" t="n"/>
@@ -5945,7 +6042,7 @@
       <c r="A384" s="1" t="n"/>
       <c r="B384" s="1" t="n"/>
       <c r="C384" s="1" t="n">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D384" s="9" t="n"/>
       <c r="E384" s="9" t="n"/>
@@ -5959,7 +6056,7 @@
       <c r="A385" s="1" t="n"/>
       <c r="B385" s="1" t="n"/>
       <c r="C385" s="1" t="n">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D385" s="9" t="n"/>
       <c r="E385" s="9" t="n"/>
@@ -5973,7 +6070,7 @@
       <c r="A386" s="1" t="n"/>
       <c r="B386" s="1" t="n"/>
       <c r="C386" s="1" t="n">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D386" s="9" t="n"/>
       <c r="E386" s="9" t="n"/>
@@ -5987,7 +6084,7 @@
       <c r="A387" s="1" t="n"/>
       <c r="B387" s="1" t="n"/>
       <c r="C387" s="1" t="n">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D387" s="9" t="n"/>
       <c r="E387" s="9" t="n"/>
@@ -6001,7 +6098,7 @@
       <c r="A388" s="1" t="n"/>
       <c r="B388" s="1" t="n"/>
       <c r="C388" s="1" t="n">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D388" s="9" t="n"/>
       <c r="E388" s="9" t="n"/>
@@ -6015,7 +6112,7 @@
       <c r="A389" s="1" t="n"/>
       <c r="B389" s="1" t="n"/>
       <c r="C389" s="1" t="n">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D389" s="9" t="n"/>
       <c r="E389" s="9" t="n"/>
@@ -6029,7 +6126,7 @@
       <c r="A390" s="1" t="n"/>
       <c r="B390" s="1" t="n"/>
       <c r="C390" s="1" t="n">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D390" s="9" t="n"/>
       <c r="E390" s="9" t="n"/>
@@ -6043,7 +6140,7 @@
       <c r="A391" s="1" t="n"/>
       <c r="B391" s="1" t="n"/>
       <c r="C391" s="1" t="n">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D391" s="9" t="n"/>
       <c r="E391" s="9" t="n"/>
@@ -6057,7 +6154,7 @@
       <c r="A392" s="1" t="n"/>
       <c r="B392" s="1" t="n"/>
       <c r="C392" s="1" t="n">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D392" s="9" t="n"/>
       <c r="E392" s="9" t="n"/>
@@ -6071,7 +6168,7 @@
       <c r="A393" s="1" t="n"/>
       <c r="B393" s="1" t="n"/>
       <c r="C393" s="1" t="n">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D393" s="9" t="n"/>
       <c r="E393" s="9" t="n"/>
@@ -6085,7 +6182,7 @@
       <c r="A394" s="1" t="n"/>
       <c r="B394" s="1" t="n"/>
       <c r="C394" s="1" t="n">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D394" s="9" t="n"/>
       <c r="E394" s="9" t="n"/>
@@ -6099,7 +6196,7 @@
       <c r="A395" s="1" t="n"/>
       <c r="B395" s="1" t="n"/>
       <c r="C395" s="1" t="n">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D395" s="9" t="n"/>
       <c r="E395" s="9" t="n"/>
@@ -6113,7 +6210,7 @@
       <c r="A396" s="1" t="n"/>
       <c r="B396" s="1" t="n"/>
       <c r="C396" s="1" t="n">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D396" s="9" t="n"/>
       <c r="E396" s="9" t="n"/>
@@ -6127,7 +6224,7 @@
       <c r="A397" s="1" t="n"/>
       <c r="B397" s="1" t="n"/>
       <c r="C397" s="1" t="n">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D397" s="9" t="n"/>
       <c r="E397" s="9" t="n"/>
@@ -6141,7 +6238,7 @@
       <c r="A398" s="1" t="n"/>
       <c r="B398" s="1" t="n"/>
       <c r="C398" s="1" t="n">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D398" s="9" t="n"/>
       <c r="E398" s="9" t="n"/>
@@ -6155,7 +6252,7 @@
       <c r="A399" s="1" t="n"/>
       <c r="B399" s="1" t="n"/>
       <c r="C399" s="1" t="n">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D399" s="9" t="n"/>
       <c r="E399" s="9" t="n"/>
@@ -6169,7 +6266,7 @@
       <c r="A400" s="1" t="n"/>
       <c r="B400" s="1" t="n"/>
       <c r="C400" s="1" t="n">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D400" s="9" t="n"/>
       <c r="E400" s="9" t="n"/>
@@ -6183,7 +6280,7 @@
       <c r="A401" s="1" t="n"/>
       <c r="B401" s="1" t="n"/>
       <c r="C401" s="1" t="n">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D401" s="9" t="n"/>
       <c r="E401" s="9" t="n"/>
@@ -6197,7 +6294,7 @@
       <c r="A402" s="1" t="n"/>
       <c r="B402" s="1" t="n"/>
       <c r="C402" s="1" t="n">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D402" s="9" t="n"/>
       <c r="E402" s="9" t="n"/>
@@ -6211,7 +6308,7 @@
       <c r="A403" s="1" t="n"/>
       <c r="B403" s="1" t="n"/>
       <c r="C403" s="1" t="n">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D403" s="9" t="n"/>
       <c r="E403" s="9" t="n"/>
@@ -6225,7 +6322,7 @@
       <c r="A404" s="1" t="n"/>
       <c r="B404" s="1" t="n"/>
       <c r="C404" s="1" t="n">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D404" s="9" t="n"/>
       <c r="E404" s="9" t="n"/>
@@ -6239,7 +6336,7 @@
       <c r="A405" s="1" t="n"/>
       <c r="B405" s="1" t="n"/>
       <c r="C405" s="1" t="n">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D405" s="9" t="n"/>
       <c r="E405" s="9" t="n"/>
@@ -6253,7 +6350,7 @@
       <c r="A406" s="1" t="n"/>
       <c r="B406" s="1" t="n"/>
       <c r="C406" s="1" t="n">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D406" s="9" t="n"/>
       <c r="E406" s="9" t="n"/>
@@ -6267,7 +6364,7 @@
       <c r="A407" s="1" t="n"/>
       <c r="B407" s="1" t="n"/>
       <c r="C407" s="1" t="n">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D407" s="9" t="n"/>
       <c r="E407" s="9" t="n"/>
@@ -6281,7 +6378,7 @@
       <c r="A408" s="1" t="n"/>
       <c r="B408" s="1" t="n"/>
       <c r="C408" s="1" t="n">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D408" s="9" t="n"/>
       <c r="E408" s="9" t="n"/>
@@ -6295,7 +6392,7 @@
       <c r="A409" s="1" t="n"/>
       <c r="B409" s="1" t="n"/>
       <c r="C409" s="1" t="n">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D409" s="9" t="n"/>
       <c r="E409" s="9" t="n"/>
@@ -6309,7 +6406,7 @@
       <c r="A410" s="1" t="n"/>
       <c r="B410" s="1" t="n"/>
       <c r="C410" s="1" t="n">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D410" s="9" t="n"/>
       <c r="E410" s="9" t="n"/>
@@ -6323,7 +6420,7 @@
       <c r="A411" s="1" t="n"/>
       <c r="B411" s="1" t="n"/>
       <c r="C411" s="1" t="n">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D411" s="9" t="n"/>
       <c r="E411" s="9" t="n"/>
@@ -6337,7 +6434,7 @@
       <c r="A412" s="1" t="n"/>
       <c r="B412" s="1" t="n"/>
       <c r="C412" s="1" t="n">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D412" s="9" t="n"/>
       <c r="E412" s="9" t="n"/>
@@ -6351,7 +6448,7 @@
       <c r="A413" s="1" t="n"/>
       <c r="B413" s="1" t="n"/>
       <c r="C413" s="1" t="n">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D413" s="9" t="n"/>
       <c r="E413" s="9" t="n"/>
@@ -6365,7 +6462,7 @@
       <c r="A414" s="1" t="n"/>
       <c r="B414" s="1" t="n"/>
       <c r="C414" s="1" t="n">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D414" s="9" t="n"/>
       <c r="E414" s="9" t="n"/>
@@ -6379,7 +6476,7 @@
       <c r="A415" s="1" t="n"/>
       <c r="B415" s="1" t="n"/>
       <c r="C415" s="1" t="n">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D415" s="9" t="n"/>
       <c r="E415" s="9" t="n"/>
@@ -6393,7 +6490,7 @@
       <c r="A416" s="1" t="n"/>
       <c r="B416" s="1" t="n"/>
       <c r="C416" s="1" t="n">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D416" s="9" t="n"/>
       <c r="E416" s="9" t="n"/>
@@ -6407,7 +6504,7 @@
       <c r="A417" s="1" t="n"/>
       <c r="B417" s="1" t="n"/>
       <c r="C417" s="1" t="n">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D417" s="9" t="n"/>
       <c r="E417" s="9" t="n"/>
@@ -6421,7 +6518,7 @@
       <c r="A418" s="1" t="n"/>
       <c r="B418" s="1" t="n"/>
       <c r="C418" s="1" t="n">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D418" s="9" t="n"/>
       <c r="E418" s="9" t="n"/>
@@ -6435,7 +6532,7 @@
       <c r="A419" s="1" t="n"/>
       <c r="B419" s="1" t="n"/>
       <c r="C419" s="1" t="n">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D419" s="9" t="n"/>
       <c r="E419" s="9" t="n"/>
@@ -6449,7 +6546,7 @@
       <c r="A420" s="1" t="n"/>
       <c r="B420" s="1" t="n"/>
       <c r="C420" s="1" t="n">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D420" s="9" t="n"/>
       <c r="E420" s="9" t="n"/>
@@ -6463,7 +6560,7 @@
       <c r="A421" s="1" t="n"/>
       <c r="B421" s="1" t="n"/>
       <c r="C421" s="1" t="n">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D421" s="9" t="n"/>
       <c r="E421" s="9" t="n"/>
@@ -6477,7 +6574,7 @@
       <c r="A422" s="1" t="n"/>
       <c r="B422" s="1" t="n"/>
       <c r="C422" s="1" t="n">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D422" s="9" t="n"/>
       <c r="E422" s="9" t="n"/>
@@ -6486,6 +6583,20 @@
       <c r="H422" s="9" t="n"/>
       <c r="I422" s="1" t="n"/>
       <c r="J422" s="1" t="n"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="1" t="n"/>
+      <c r="B423" s="1" t="n"/>
+      <c r="C423" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="D423" s="9" t="n"/>
+      <c r="E423" s="9" t="n"/>
+      <c r="F423" s="9" t="n"/>
+      <c r="G423" s="6" t="n"/>
+      <c r="H423" s="9" t="n"/>
+      <c r="I423" s="1" t="n"/>
+      <c r="J423" s="1" t="n"/>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>